<commit_message>
Add April 2025 newsletter content and update resident directory
</commit_message>
<xml_diff>
--- a/3-1-heritage/0-heritage-happenings/2025/04-april-hh/resident-directory/2025-04-heritage-resident-directory.xlsx
+++ b/3-1-heritage/0-heritage-happenings/2025/04-april-hh/resident-directory/2025-04-heritage-resident-directory.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4348e1419f457eb2/Documents/GitHub/theo-armour-agenda/3-1-heritage/0-heritage-happenings/2025/04-april-hh/resident-directory/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="958" documentId="8_{47523533-A004-48EF-BEEC-0FA3DE3C4717}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{54C3799A-19EA-4529-8AAC-C333C5293197}"/>
+  <xr:revisionPtr revIDLastSave="970" documentId="8_{47523533-A004-48EF-BEEC-0FA3DE3C4717}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{48DF991E-94E1-424A-8471-F753BE537874}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="754" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="754" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Residents" sheetId="1" r:id="rId1"/>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1854" uniqueCount="1185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1830" uniqueCount="1164">
   <si>
     <t>First Name</t>
   </si>
@@ -2340,12 +2340,6 @@
     <t>David</t>
   </si>
   <si>
-    <t>Burnett</t>
-  </si>
-  <si>
-    <t>&lt;ddburnett@gmail.com&gt;</t>
-  </si>
-  <si>
     <t>Morgan</t>
   </si>
   <si>
@@ -2550,15 +2544,6 @@
     <t>&lt;santani@gmail.com&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">Shammah </t>
-  </si>
-  <si>
-    <t>Chancellor</t>
-  </si>
-  <si>
-    <t>&lt;shammah.chancellor@gmail.com&gt;</t>
-  </si>
-  <si>
     <t>Stephen</t>
   </si>
   <si>
@@ -2634,15 +2619,6 @@
     <t>&lt;bennet.engelhardt@gmail.com&gt;</t>
   </si>
   <si>
-    <t>Jerome</t>
-  </si>
-  <si>
-    <t>Tavé</t>
-  </si>
-  <si>
-    <t>&lt;jerometave@gmail.com&gt;</t>
-  </si>
-  <si>
     <t>Arvind</t>
   </si>
   <si>
@@ -2667,15 +2643,6 @@
     <t>&lt;ray94903@gmail.com&gt;</t>
   </si>
   <si>
-    <t>Manfred</t>
-  </si>
-  <si>
-    <t>MacKeben</t>
-  </si>
-  <si>
-    <t>&lt;manfred.mackeben@gmail.com&gt;</t>
-  </si>
-  <si>
     <t>Olga</t>
   </si>
   <si>
@@ -2694,12 +2661,6 @@
     <t>Jon</t>
   </si>
   <si>
-    <t>Rubin</t>
-  </si>
-  <si>
-    <t>&lt;jonrubin6@gmail.com&gt;</t>
-  </si>
-  <si>
     <t>Merrill</t>
   </si>
   <si>
@@ -2719,30 +2680,6 @@
   </si>
   <si>
     <t>&lt;mwfarmcsa@gmail.com&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Richard </t>
-  </si>
-  <si>
-    <t>Dewath</t>
-  </si>
-  <si>
-    <t>&lt;dewath@gmail.com&gt;</t>
-  </si>
-  <si>
-    <t>Sunil</t>
-  </si>
-  <si>
-    <t>Moothedath</t>
-  </si>
-  <si>
-    <t>&lt;sunil@c4h3i.com&gt;</t>
-  </si>
-  <si>
-    <t>Price</t>
-  </si>
-  <si>
-    <t>&lt;tprice41@gmail.com&gt;</t>
   </si>
   <si>
     <t>Alumni</t>
@@ -4482,9 +4419,9 @@
   </sheetPr>
   <dimension ref="A1:I1005"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K8" sqref="K8"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A66" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F2" sqref="F2:F74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.15234375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -4502,7 +4439,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="17" t="s">
-        <v>1074</v>
+        <v>1053</v>
       </c>
       <c r="B1" s="17" t="s">
         <v>1</v>
@@ -4612,20 +4549,20 @@
     </row>
     <row r="5" spans="1:9" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A5" s="17" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>1182</v>
+        <v>1161</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1" t="s">
         <v>38</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>1183</v>
-      </c>
-      <c r="F5" s="39" t="s">
-        <v>1184</v>
+        <v>1162</v>
+      </c>
+      <c r="F5" s="40" t="s">
+        <v>1163</v>
       </c>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
@@ -5035,10 +4972,10 @@
     </row>
     <row r="22" spans="1:9" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A22" s="17" t="s">
-        <v>1014</v>
+        <v>993</v>
       </c>
       <c r="B22" s="17" t="s">
-        <v>1015</v>
+        <v>994</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>19</v>
@@ -5047,10 +4984,10 @@
         <v>38</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>1016</v>
+        <v>995</v>
       </c>
       <c r="F22" s="40" t="s">
-        <v>1018</v>
+        <v>997</v>
       </c>
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
@@ -5250,7 +5187,7 @@
         <v>19</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>1103</v>
+        <v>1082</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>163</v>
@@ -5570,7 +5507,7 @@
         <v>19</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>1094</v>
+        <v>1073</v>
       </c>
       <c r="E43" s="1" t="s">
         <v>231</v>
@@ -5587,7 +5524,7 @@
     </row>
     <row r="44" spans="1:9" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A44" s="17" t="s">
-        <v>1049</v>
+        <v>1028</v>
       </c>
       <c r="B44" s="17" t="s">
         <v>233</v>
@@ -5801,42 +5738,42 @@
     </row>
     <row r="53" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="17" t="s">
-        <v>1095</v>
+        <v>1074</v>
       </c>
       <c r="B53" s="17" t="s">
-        <v>1096</v>
+        <v>1075</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>1097</v>
+        <v>1076</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>1098</v>
+        <v>1077</v>
       </c>
       <c r="F53" s="39" t="s">
-        <v>1099</v>
+        <v>1078</v>
       </c>
       <c r="I53" s="53" t="s">
-        <v>1100</v>
+        <v>1079</v>
       </c>
     </row>
     <row r="54" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="17" t="s">
-        <v>848</v>
+        <v>843</v>
       </c>
       <c r="B54" s="17" t="s">
-        <v>1096</v>
+        <v>1075</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>1097</v>
+        <v>1076</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>1101</v>
+        <v>1080</v>
       </c>
       <c r="F54" s="40" t="s">
-        <v>1104</v>
+        <v>1083</v>
       </c>
       <c r="I54" s="53" t="s">
-        <v>1102</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="55" spans="1:9" ht="13.5" x14ac:dyDescent="0.3">
@@ -5885,7 +5822,7 @@
         <v>288</v>
       </c>
       <c r="F56" s="49" t="s">
-        <v>1073</v>
+        <v>1052</v>
       </c>
       <c r="G56" s="1"/>
       <c r="H56" s="1"/>
@@ -9169,9 +9106,10 @@
     <hyperlink ref="F56" r:id="rId5" xr:uid="{EA80CD83-9791-49E5-9CC4-F2AA9892E575}"/>
     <hyperlink ref="F22" r:id="rId6" xr:uid="{DFF8D86C-B09F-4E2D-97B8-F45B63E33AAA}"/>
     <hyperlink ref="F54" r:id="rId7" display="jmnaughton1946@gmail.com" xr:uid="{A7FBD182-2FD6-410C-9DE6-4164C35EF8C5}"/>
+    <hyperlink ref="F5" r:id="rId8" xr:uid="{4263E288-467C-448D-8E0B-84857F5A2A39}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="86" fitToHeight="0" orientation="landscape" r:id="rId8"/>
+  <pageSetup scale="86" fitToHeight="0" orientation="landscape" r:id="rId9"/>
 </worksheet>
 </file>
 
@@ -9224,7 +9162,7 @@
     </row>
     <row r="3" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>1075</v>
+        <v>1054</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>17</v>
@@ -11432,7 +11370,7 @@
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A79" s="11" t="s">
-        <v>1017</v>
+        <v>996</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.35">
@@ -11451,7 +11389,7 @@
     </row>
     <row r="82" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A82" s="52" t="s">
-        <v>1082</v>
+        <v>1061</v>
       </c>
       <c r="B82" s="52"/>
       <c r="C82" s="52"/>
@@ -12690,7 +12628,7 @@
   <sheetData>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>1138</v>
+        <v>1117</v>
       </c>
       <c r="B2" t="s">
         <v>174</v>
@@ -12698,7 +12636,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>1142</v>
+        <v>1121</v>
       </c>
       <c r="B3" t="s">
         <v>174</v>
@@ -12706,7 +12644,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>1176</v>
+        <v>1155</v>
       </c>
       <c r="B4" t="s">
         <v>174</v>
@@ -12714,7 +12652,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>1181</v>
+        <v>1160</v>
       </c>
       <c r="B5" t="s">
         <v>174</v>
@@ -12722,7 +12660,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>1124</v>
+        <v>1103</v>
       </c>
       <c r="B6" t="s">
         <v>110</v>
@@ -12730,7 +12668,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>1135</v>
+        <v>1114</v>
       </c>
       <c r="B7" t="s">
         <v>160</v>
@@ -12738,7 +12676,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>1129</v>
+        <v>1108</v>
       </c>
       <c r="B8" t="s">
         <v>132</v>
@@ -12746,7 +12684,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>1164</v>
+        <v>1143</v>
       </c>
       <c r="B9" t="s">
         <v>301</v>
@@ -12754,7 +12692,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>1147</v>
+        <v>1126</v>
       </c>
       <c r="B10" t="s">
         <v>222</v>
@@ -12762,7 +12700,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>1175</v>
+        <v>1154</v>
       </c>
       <c r="B11" t="s">
         <v>222</v>
@@ -12770,7 +12708,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>1111</v>
+        <v>1090</v>
       </c>
       <c r="B12" t="s">
         <v>35</v>
@@ -12778,15 +12716,15 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>1159</v>
+        <v>1138</v>
       </c>
       <c r="B13" t="s">
-        <v>1100</v>
+        <v>1079</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>1127</v>
+        <v>1106</v>
       </c>
       <c r="B14" t="s">
         <v>127</v>
@@ -12794,7 +12732,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>1172</v>
+        <v>1151</v>
       </c>
       <c r="B15" t="s">
         <v>127</v>
@@ -12802,7 +12740,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>1128</v>
+        <v>1107</v>
       </c>
       <c r="B16" t="s">
         <v>342</v>
@@ -12810,7 +12748,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>1171</v>
+        <v>1150</v>
       </c>
       <c r="B17" t="s">
         <v>342</v>
@@ -12818,7 +12756,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>1148</v>
+        <v>1127</v>
       </c>
       <c r="B18" t="s">
         <v>228</v>
@@ -12826,7 +12764,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>1144</v>
+        <v>1123</v>
       </c>
       <c r="B19" t="s">
         <v>208</v>
@@ -12834,7 +12772,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>1125</v>
+        <v>1104</v>
       </c>
       <c r="B20" t="s">
         <v>116</v>
@@ -12842,15 +12780,15 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>1160</v>
+        <v>1139</v>
       </c>
       <c r="B21" t="s">
-        <v>1102</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>1163</v>
+        <v>1142</v>
       </c>
       <c r="B22" t="s">
         <v>295</v>
@@ -12858,7 +12796,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>1121</v>
+        <v>1100</v>
       </c>
       <c r="B23" t="s">
         <v>94</v>
@@ -12866,7 +12804,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>1116</v>
+        <v>1095</v>
       </c>
       <c r="B24" t="s">
         <v>62</v>
@@ -12874,7 +12812,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>1166</v>
+        <v>1145</v>
       </c>
       <c r="B25" t="s">
         <v>312</v>
@@ -12882,7 +12820,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>1174</v>
+        <v>1153</v>
       </c>
       <c r="B26" t="s">
         <v>355</v>
@@ -12890,7 +12828,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>1167</v>
+        <v>1146</v>
       </c>
       <c r="B27" t="s">
         <v>317</v>
@@ -12898,7 +12836,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>1168</v>
+        <v>1147</v>
       </c>
       <c r="B28" t="s">
         <v>327</v>
@@ -12906,7 +12844,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>1162</v>
+        <v>1141</v>
       </c>
       <c r="B29" t="s">
         <v>289</v>
@@ -12914,7 +12852,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>1137</v>
+        <v>1116</v>
       </c>
       <c r="B30" t="s">
         <v>170</v>
@@ -12922,7 +12860,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>1140</v>
+        <v>1119</v>
       </c>
       <c r="B31" t="s">
         <v>186</v>
@@ -12930,7 +12868,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>1177</v>
+        <v>1156</v>
       </c>
       <c r="B32" t="s">
         <v>369</v>
@@ -12938,7 +12876,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>1139</v>
+        <v>1118</v>
       </c>
       <c r="B33" t="s">
         <v>180</v>
@@ -12946,7 +12884,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>1119</v>
+        <v>1098</v>
       </c>
       <c r="B34" t="s">
         <v>84</v>
@@ -12954,7 +12892,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>1123</v>
+        <v>1102</v>
       </c>
       <c r="B35" t="s">
         <v>104</v>
@@ -12962,7 +12900,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>1170</v>
+        <v>1149</v>
       </c>
       <c r="B36" t="s">
         <v>336</v>
@@ -12970,7 +12908,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>1130</v>
+        <v>1109</v>
       </c>
       <c r="B37" t="s">
         <v>135</v>
@@ -12978,7 +12916,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>1132</v>
+        <v>1111</v>
       </c>
       <c r="B38" t="s">
         <v>147</v>
@@ -12986,7 +12924,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>1149</v>
+        <v>1128</v>
       </c>
       <c r="B39" t="s">
         <v>147</v>
@@ -12994,7 +12932,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>1179</v>
+        <v>1158</v>
       </c>
       <c r="B40" t="s">
         <v>381</v>
@@ -13002,7 +12940,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>1113</v>
+        <v>1092</v>
       </c>
       <c r="B41" t="s">
         <v>47</v>
@@ -13010,7 +12948,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>1156</v>
+        <v>1135</v>
       </c>
       <c r="B42" t="s">
         <v>268</v>
@@ -13018,7 +12956,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>1146</v>
+        <v>1125</v>
       </c>
       <c r="B43" t="s">
         <v>219</v>
@@ -13026,7 +12964,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>1145</v>
+        <v>1124</v>
       </c>
       <c r="B44" t="s">
         <v>213</v>
@@ -13034,7 +12972,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>1117</v>
+        <v>1096</v>
       </c>
       <c r="B45" t="s">
         <v>68</v>
@@ -13042,7 +12980,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>1151</v>
+        <v>1130</v>
       </c>
       <c r="B46" t="s">
         <v>68</v>
@@ -13050,7 +12988,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>1169</v>
+        <v>1148</v>
       </c>
       <c r="B47" t="s">
         <v>332</v>
@@ -13058,7 +12996,7 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>1153</v>
+        <v>1132</v>
       </c>
       <c r="B48" t="s">
         <v>252</v>
@@ -13066,7 +13004,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>1109</v>
+        <v>1088</v>
       </c>
       <c r="B49" t="s">
         <v>16</v>
@@ -13074,7 +13012,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>1157</v>
+        <v>1136</v>
       </c>
       <c r="B50" t="s">
         <v>273</v>
@@ -13082,7 +13020,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>1118</v>
+        <v>1097</v>
       </c>
       <c r="B51" t="s">
         <v>79</v>
@@ -13090,7 +13028,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>1110</v>
+        <v>1089</v>
       </c>
       <c r="B52" t="s">
         <v>29</v>
@@ -13098,7 +13036,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>1178</v>
+        <v>1157</v>
       </c>
       <c r="B53" t="s">
         <v>374</v>
@@ -13106,7 +13044,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>1141</v>
+        <v>1120</v>
       </c>
       <c r="B54" t="s">
         <v>192</v>
@@ -13114,7 +13052,7 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>1114</v>
+        <v>1093</v>
       </c>
       <c r="B55" t="s">
         <v>54</v>
@@ -13122,7 +13060,7 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>1161</v>
+        <v>1140</v>
       </c>
       <c r="B56" t="s">
         <v>54</v>
@@ -13130,7 +13068,7 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>1131</v>
+        <v>1110</v>
       </c>
       <c r="B57" t="s">
         <v>141</v>
@@ -13138,7 +13076,7 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>1143</v>
+        <v>1122</v>
       </c>
       <c r="B58" t="s">
         <v>203</v>
@@ -13146,7 +13084,7 @@
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>1115</v>
+        <v>1094</v>
       </c>
       <c r="B59" t="s">
         <v>56</v>
@@ -13154,7 +13092,7 @@
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>1158</v>
+        <v>1137</v>
       </c>
       <c r="B60" t="s">
         <v>277</v>
@@ -13162,7 +13100,7 @@
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>1133</v>
+        <v>1112</v>
       </c>
       <c r="B61" t="s">
         <v>152</v>
@@ -13170,7 +13108,7 @@
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>1134</v>
+        <v>1113</v>
       </c>
       <c r="B62" t="s">
         <v>154</v>
@@ -13178,7 +13116,7 @@
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>1126</v>
+        <v>1105</v>
       </c>
       <c r="B63" t="s">
         <v>122</v>
@@ -13186,7 +13124,7 @@
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>1112</v>
+        <v>1091</v>
       </c>
       <c r="B64" t="s">
         <v>41</v>
@@ -13194,7 +13132,7 @@
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>1180</v>
+        <v>1159</v>
       </c>
       <c r="B65" t="s">
         <v>385</v>
@@ -13202,7 +13140,7 @@
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>1165</v>
+        <v>1144</v>
       </c>
       <c r="B66" t="s">
         <v>306</v>
@@ -13210,7 +13148,7 @@
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>1154</v>
+        <v>1133</v>
       </c>
       <c r="B67" t="s">
         <v>257</v>
@@ -13218,7 +13156,7 @@
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>1173</v>
+        <v>1152</v>
       </c>
       <c r="B68" t="s">
         <v>257</v>
@@ -13226,7 +13164,7 @@
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>1136</v>
+        <v>1115</v>
       </c>
       <c r="B69" t="s">
         <v>165</v>
@@ -13234,7 +13172,7 @@
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>1155</v>
+        <v>1134</v>
       </c>
       <c r="B70" t="s">
         <v>165</v>
@@ -13242,7 +13180,7 @@
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>1150</v>
+        <v>1129</v>
       </c>
       <c r="B71" t="s">
         <v>237</v>
@@ -13250,7 +13188,7 @@
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>1122</v>
+        <v>1101</v>
       </c>
       <c r="B72" t="s">
         <v>99</v>
@@ -13258,7 +13196,7 @@
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>1120</v>
+        <v>1099</v>
       </c>
       <c r="B73" t="s">
         <v>90</v>
@@ -13266,7 +13204,7 @@
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>1152</v>
+        <v>1131</v>
       </c>
       <c r="B74" t="s">
         <v>247</v>
@@ -13286,7 +13224,7 @@
   <dimension ref="A1:E100"/>
   <sheetViews>
     <sheetView showWhiteSpace="0" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C2" sqref="C2:C62"/>
     </sheetView>
   </sheetViews>
@@ -13302,19 +13240,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="27" t="s">
-        <v>1074</v>
+        <v>1053</v>
       </c>
       <c r="B1" s="27" t="s">
-        <v>1019</v>
+        <v>998</v>
       </c>
       <c r="C1" s="20" t="s">
         <v>5</v>
       </c>
       <c r="D1" s="27" t="s">
-        <v>1020</v>
+        <v>999</v>
       </c>
       <c r="E1" s="27" t="s">
-        <v>1021</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
@@ -13339,13 +13277,13 @@
         <v>748</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>1055</v>
+        <v>1034</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>1054</v>
+        <v>1033</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>1053</v>
+        <v>1032</v>
       </c>
       <c r="E3" s="11" t="s">
         <v>25</v>
@@ -13379,10 +13317,10 @@
         <v>639</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>1028</v>
+        <v>1007</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>1029</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
@@ -13441,7 +13379,7 @@
         <v>645</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>1040</v>
+        <v>1019</v>
       </c>
       <c r="C9" s="19" t="s">
         <v>646</v>
@@ -13458,7 +13396,7 @@
         <v>647</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>1022</v>
+        <v>1001</v>
       </c>
       <c r="C10" s="19" t="s">
         <v>648</v>
@@ -13498,7 +13436,7 @@
         <v>652</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>1032</v>
+        <v>1011</v>
       </c>
       <c r="E12" s="11" t="s">
         <v>143</v>
@@ -13574,7 +13512,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="11" t="s">
-        <v>1033</v>
+        <v>1012</v>
       </c>
       <c r="B17" s="11" t="s">
         <v>166</v>
@@ -13679,16 +13617,16 @@
         <v>661</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>1023</v>
+        <v>1002</v>
       </c>
       <c r="C23" s="19" t="s">
-        <v>1024</v>
+        <v>1003</v>
       </c>
       <c r="D23" s="11" t="s">
         <v>171</v>
       </c>
       <c r="E23" s="11" t="s">
-        <v>1025</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
@@ -13696,7 +13634,7 @@
         <v>662</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>1023</v>
+        <v>1002</v>
       </c>
       <c r="C24" s="19" t="s">
         <v>663</v>
@@ -13705,18 +13643,18 @@
         <v>171</v>
       </c>
       <c r="E24" s="11" t="s">
-        <v>1025</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="38" t="s">
-        <v>1050</v>
+        <v>1029</v>
       </c>
       <c r="B25" s="38" t="s">
         <v>188</v>
       </c>
       <c r="C25" s="38" t="s">
-        <v>1051</v>
+        <v>1030</v>
       </c>
       <c r="D25" s="19" t="s">
         <v>187</v>
@@ -13733,7 +13671,7 @@
         <v>188</v>
       </c>
       <c r="C26" s="38" t="s">
-        <v>1052</v>
+        <v>1031</v>
       </c>
       <c r="D26" s="19" t="s">
         <v>187</v>
@@ -13747,7 +13685,7 @@
         <v>664</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>1037</v>
+        <v>1016</v>
       </c>
       <c r="C27" s="19" t="s">
         <v>665</v>
@@ -13818,7 +13756,7 @@
         <v>230</v>
       </c>
       <c r="C31" s="19" t="s">
-        <v>1034</v>
+        <v>1013</v>
       </c>
       <c r="D31" s="11" t="s">
         <v>229</v>
@@ -13829,16 +13767,16 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" s="11" t="s">
-        <v>1057</v>
+        <v>1036</v>
       </c>
       <c r="B32" s="11" t="s">
         <v>233</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>1056</v>
+        <v>1035</v>
       </c>
       <c r="D32" s="11" t="s">
-        <v>1049</v>
+        <v>1028</v>
       </c>
       <c r="E32" s="11" t="s">
         <v>233</v>
@@ -13846,13 +13784,13 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" s="11" t="s">
-        <v>1062</v>
+        <v>1041</v>
       </c>
       <c r="B33" s="11" t="s">
         <v>249</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>1061</v>
+        <v>1040</v>
       </c>
       <c r="D33" s="11" t="s">
         <v>248</v>
@@ -13897,13 +13835,13 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" s="11" t="s">
-        <v>1058</v>
+        <v>1037</v>
       </c>
       <c r="B36" s="11" t="s">
-        <v>1059</v>
+        <v>1038</v>
       </c>
       <c r="C36" s="11" t="s">
-        <v>1060</v>
+        <v>1039</v>
       </c>
       <c r="D36" s="11" t="s">
         <v>258</v>
@@ -13968,13 +13906,13 @@
         <v>684</v>
       </c>
       <c r="B40" s="11" t="s">
-        <v>1026</v>
+        <v>1005</v>
       </c>
       <c r="C40" s="19" t="s">
         <v>685</v>
       </c>
       <c r="D40" s="11" t="s">
-        <v>1027</v>
+        <v>1006</v>
       </c>
       <c r="E40" s="11" t="s">
         <v>270</v>
@@ -13991,7 +13929,7 @@
         <v>683</v>
       </c>
       <c r="D41" s="11" t="s">
-        <v>1027</v>
+        <v>1006</v>
       </c>
       <c r="E41" s="11" t="s">
         <v>270</v>
@@ -14008,7 +13946,7 @@
         <v>682</v>
       </c>
       <c r="D42" s="11" t="s">
-        <v>1027</v>
+        <v>1006</v>
       </c>
       <c r="E42" s="11" t="s">
         <v>270</v>
@@ -14019,13 +13957,13 @@
         <v>193</v>
       </c>
       <c r="B43" s="11" t="s">
-        <v>1036</v>
+        <v>1015</v>
       </c>
       <c r="C43" s="38" t="s">
-        <v>1076</v>
+        <v>1055</v>
       </c>
       <c r="D43" s="11" t="s">
-        <v>1027</v>
+        <v>1006</v>
       </c>
       <c r="E43" s="11" t="s">
         <v>270</v>
@@ -14076,7 +14014,7 @@
         <v>690</v>
       </c>
       <c r="D46" s="11" t="s">
-        <v>1041</v>
+        <v>1020</v>
       </c>
       <c r="E46" s="11" t="s">
         <v>283</v>
@@ -14093,7 +14031,7 @@
         <v>692</v>
       </c>
       <c r="D47" s="11" t="s">
-        <v>1041</v>
+        <v>1020</v>
       </c>
       <c r="E47" s="11" t="s">
         <v>283</v>
@@ -14104,13 +14042,13 @@
         <v>693</v>
       </c>
       <c r="B48" s="11" t="s">
-        <v>1042</v>
+        <v>1021</v>
       </c>
       <c r="C48" s="19" t="s">
         <v>694</v>
       </c>
       <c r="D48" s="11" t="s">
-        <v>1041</v>
+        <v>1020</v>
       </c>
       <c r="E48" s="11" t="s">
         <v>283</v>
@@ -14141,7 +14079,7 @@
         <v>297</v>
       </c>
       <c r="C50" s="38" t="s">
-        <v>1077</v>
+        <v>1056</v>
       </c>
       <c r="D50" s="11" t="s">
         <v>296</v>
@@ -14172,7 +14110,7 @@
         <v>701</v>
       </c>
       <c r="B52" s="11" t="s">
-        <v>1038</v>
+        <v>1017</v>
       </c>
       <c r="C52" s="19" t="s">
         <v>702</v>
@@ -14186,7 +14124,7 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A53" s="11" t="s">
-        <v>1043</v>
+        <v>1022</v>
       </c>
       <c r="B53" s="11" t="s">
         <v>314</v>
@@ -14240,7 +14178,7 @@
         <v>706</v>
       </c>
       <c r="B56" s="11" t="s">
-        <v>1035</v>
+        <v>1014</v>
       </c>
       <c r="C56" s="19" t="s">
         <v>707</v>
@@ -14254,10 +14192,10 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A57" s="11" t="s">
-        <v>806</v>
+        <v>804</v>
       </c>
       <c r="B57" s="11" t="s">
-        <v>1039</v>
+        <v>1018</v>
       </c>
       <c r="C57" s="19" t="s">
         <v>705</v>
@@ -14311,10 +14249,10 @@
         <v>719</v>
       </c>
       <c r="C60" s="38" t="s">
-        <v>1030</v>
+        <v>1009</v>
       </c>
       <c r="D60" s="11" t="s">
-        <v>1031</v>
+        <v>1010</v>
       </c>
       <c r="E60" s="11" t="s">
         <v>376</v>
@@ -14331,7 +14269,7 @@
         <v>717</v>
       </c>
       <c r="D61" s="11" t="s">
-        <v>1031</v>
+        <v>1010</v>
       </c>
       <c r="E61" s="11" t="s">
         <v>376</v>
@@ -14348,7 +14286,7 @@
         <v>715</v>
       </c>
       <c r="D62" s="11" t="s">
-        <v>1031</v>
+        <v>1010</v>
       </c>
       <c r="E62" s="11" t="s">
         <v>376</v>
@@ -14743,7 +14681,7 @@
         <v>233</v>
       </c>
       <c r="B24" s="48" t="s">
-        <v>1049</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
@@ -14859,9 +14797,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CAA4147-474C-47CD-A0DD-4C67000E8368}">
   <dimension ref="A1:C75"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E70" sqref="E70"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C13" sqref="A13:C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23046875" defaultRowHeight="17.5" x14ac:dyDescent="0.35"/>
@@ -14877,7 +14815,7 @@
   <sheetData>
     <row r="1" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="13" t="s">
-        <v>1074</v>
+        <v>1053</v>
       </c>
       <c r="B1" s="13" t="s">
         <v>622</v>
@@ -14888,24 +14826,24 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="11" t="s">
-        <v>860</v>
+        <v>852</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>861</v>
+        <v>853</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>862</v>
+        <v>854</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="11" t="s">
-        <v>868</v>
+        <v>857</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>869</v>
+        <v>858</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>870</v>
+        <v>859</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
@@ -14943,7 +14881,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="8" t="s">
-        <v>1047</v>
+        <v>1026</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>31</v>
@@ -14965,18 +14903,18 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="11" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="B9" s="11" t="s">
         <v>31</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="11" t="s">
-        <v>1048</v>
+        <v>1027</v>
       </c>
       <c r="B10" s="11" t="s">
         <v>743</v>
@@ -14987,46 +14925,35 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="11" t="s">
-        <v>832</v>
+        <v>827</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>833</v>
+        <v>828</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>834</v>
+        <v>829</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="11" t="s">
-        <v>842</v>
+        <v>837</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>843</v>
+        <v>838</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>844</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A13" s="11" t="s">
-        <v>755</v>
-      </c>
-      <c r="B13" s="11" t="s">
-        <v>756</v>
-      </c>
-      <c r="C13" s="11" t="s">
-        <v>757</v>
+        <v>839</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="11" t="s">
+        <v>775</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>776</v>
+      </c>
+      <c r="C14" s="11" t="s">
         <v>777</v>
-      </c>
-      <c r="B14" s="11" t="s">
-        <v>778</v>
-      </c>
-      <c r="C14" s="11" t="s">
-        <v>779</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
@@ -15034,21 +14961,21 @@
         <v>728</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="11" t="s">
+        <v>790</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>791</v>
+      </c>
+      <c r="C16" s="11" t="s">
         <v>792</v>
-      </c>
-      <c r="B16" s="11" t="s">
-        <v>793</v>
-      </c>
-      <c r="C16" s="11" t="s">
-        <v>794</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
@@ -15062,26 +14989,15 @@
         <v>754</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A18" s="11" t="s">
-        <v>826</v>
-      </c>
-      <c r="B18" s="11" t="s">
-        <v>827</v>
-      </c>
-      <c r="C18" s="11" t="s">
-        <v>828</v>
-      </c>
-    </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="11" t="s">
-        <v>829</v>
+        <v>824</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>830</v>
+        <v>825</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>831</v>
+        <v>826</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
@@ -15089,109 +15005,98 @@
         <v>290</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>802</v>
+        <v>800</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="11" t="s">
-        <v>835</v>
+        <v>830</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>836</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A22" s="11" t="s">
-        <v>883</v>
-      </c>
-      <c r="B22" s="11" t="s">
-        <v>884</v>
-      </c>
-      <c r="C22" s="11" t="s">
-        <v>885</v>
+        <v>831</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="11" t="s">
-        <v>1005</v>
+        <v>984</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>1006</v>
+        <v>985</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>1007</v>
+        <v>986</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" s="11" t="s">
+        <v>766</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>767</v>
+      </c>
+      <c r="C24" s="11" t="s">
         <v>768</v>
-      </c>
-      <c r="B24" s="11" t="s">
-        <v>769</v>
-      </c>
-      <c r="C24" s="11" t="s">
-        <v>770</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" s="11" t="s">
-        <v>817</v>
+        <v>815</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>863</v>
+        <v>855</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>864</v>
+        <v>856</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" s="11" t="s">
-        <v>845</v>
+        <v>840</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>846</v>
+        <v>841</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>847</v>
+        <v>842</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" s="11" t="s">
+        <v>772</v>
+      </c>
+      <c r="B27" s="11" t="s">
+        <v>773</v>
+      </c>
+      <c r="C27" s="11" t="s">
         <v>774</v>
-      </c>
-      <c r="B27" s="11" t="s">
-        <v>775</v>
-      </c>
-      <c r="C27" s="11" t="s">
-        <v>776</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" s="11" t="s">
-        <v>813</v>
+        <v>811</v>
       </c>
       <c r="B28" s="11" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" s="11" t="s">
-        <v>851</v>
+        <v>846</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>852</v>
+        <v>847</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>853</v>
+        <v>848</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
@@ -15199,87 +15104,87 @@
         <v>389</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>763</v>
+        <v>761</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>764</v>
+        <v>762</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" s="11" t="s">
+        <v>780</v>
+      </c>
+      <c r="B31" s="11" t="s">
+        <v>781</v>
+      </c>
+      <c r="C31" s="11" t="s">
         <v>782</v>
-      </c>
-      <c r="B31" s="11" t="s">
-        <v>783</v>
-      </c>
-      <c r="C31" s="11" t="s">
-        <v>784</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" s="11" t="s">
-        <v>795</v>
+        <v>793</v>
       </c>
       <c r="B32" s="11" t="s">
-        <v>871</v>
+        <v>860</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>872</v>
+        <v>861</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" s="11" t="s">
+        <v>793</v>
+      </c>
+      <c r="B33" s="11" t="s">
+        <v>794</v>
+      </c>
+      <c r="C33" s="11" t="s">
         <v>795</v>
-      </c>
-      <c r="B33" s="11" t="s">
-        <v>796</v>
-      </c>
-      <c r="C33" s="11" t="s">
-        <v>797</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" s="11" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="B34" s="11" t="s">
         <v>137</v>
       </c>
       <c r="C34" s="11" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" s="11" t="s">
+        <v>763</v>
+      </c>
+      <c r="B35" s="11" t="s">
+        <v>764</v>
+      </c>
+      <c r="C35" s="11" t="s">
         <v>765</v>
-      </c>
-      <c r="B35" s="11" t="s">
-        <v>766</v>
-      </c>
-      <c r="C35" s="11" t="s">
-        <v>767</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" s="11" t="s">
+        <v>801</v>
+      </c>
+      <c r="B36" s="11" t="s">
+        <v>802</v>
+      </c>
+      <c r="C36" s="11" t="s">
         <v>803</v>
-      </c>
-      <c r="B36" s="11" t="s">
-        <v>804</v>
-      </c>
-      <c r="C36" s="11" t="s">
-        <v>805</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" s="11" t="s">
+        <v>758</v>
+      </c>
+      <c r="B37" s="11" t="s">
+        <v>759</v>
+      </c>
+      <c r="C37" s="11" t="s">
         <v>760</v>
-      </c>
-      <c r="B37" s="11" t="s">
-        <v>761</v>
-      </c>
-      <c r="C37" s="11" t="s">
-        <v>762</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.35">
@@ -15304,26 +15209,15 @@
         <v>747</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A40" s="11" t="s">
-        <v>865</v>
-      </c>
-      <c r="B40" s="11" t="s">
-        <v>866</v>
-      </c>
-      <c r="C40" s="11" t="s">
-        <v>867</v>
-      </c>
-    </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" s="11" t="s">
-        <v>880</v>
+        <v>867</v>
       </c>
       <c r="B41" s="11" t="s">
-        <v>881</v>
+        <v>868</v>
       </c>
       <c r="C41" s="11" t="s">
-        <v>882</v>
+        <v>869</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.35">
@@ -15331,10 +15225,10 @@
         <v>672</v>
       </c>
       <c r="B42" s="11" t="s">
-        <v>1008</v>
+        <v>987</v>
       </c>
       <c r="C42" s="11" t="s">
-        <v>1009</v>
+        <v>988</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.35">
@@ -15342,10 +15236,10 @@
         <v>651</v>
       </c>
       <c r="B43" s="11" t="s">
-        <v>876</v>
+        <v>863</v>
       </c>
       <c r="C43" s="11" t="s">
-        <v>877</v>
+        <v>864</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.35">
@@ -15361,35 +15255,24 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" s="11" t="s">
-        <v>848</v>
+        <v>843</v>
       </c>
       <c r="B45" s="11" t="s">
-        <v>849</v>
+        <v>844</v>
       </c>
       <c r="C45" s="11" t="s">
-        <v>850</v>
+        <v>845</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46" s="11" t="s">
-        <v>811</v>
+        <v>809</v>
       </c>
       <c r="B46" s="11" t="s">
         <v>249</v>
       </c>
       <c r="C46" s="38" t="s">
-        <v>812</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A47" s="11" t="s">
-        <v>886</v>
-      </c>
-      <c r="B47" s="11" t="s">
-        <v>887</v>
-      </c>
-      <c r="C47" s="11" t="s">
-        <v>888</v>
+        <v>810</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.35">
@@ -15397,21 +15280,21 @@
         <v>755</v>
       </c>
       <c r="B48" s="11" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="C48" s="11" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49" s="11" t="s">
-        <v>815</v>
+        <v>813</v>
       </c>
       <c r="B49" s="11" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="C49" s="11" t="s">
-        <v>816</v>
+        <v>814</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.35">
@@ -15419,43 +15302,43 @@
         <v>9</v>
       </c>
       <c r="B50" s="11" t="s">
-        <v>809</v>
+        <v>807</v>
       </c>
       <c r="C50" s="11" t="s">
-        <v>810</v>
+        <v>808</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51" s="11" t="s">
+        <v>769</v>
+      </c>
+      <c r="B51" s="11" t="s">
+        <v>770</v>
+      </c>
+      <c r="C51" s="11" t="s">
         <v>771</v>
-      </c>
-      <c r="B51" s="11" t="s">
-        <v>772</v>
-      </c>
-      <c r="C51" s="11" t="s">
-        <v>773</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52" s="11" t="s">
+        <v>804</v>
+      </c>
+      <c r="B52" s="11" t="s">
+        <v>805</v>
+      </c>
+      <c r="C52" s="11" t="s">
         <v>806</v>
-      </c>
-      <c r="B52" s="11" t="s">
-        <v>807</v>
-      </c>
-      <c r="C52" s="11" t="s">
-        <v>808</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53" s="11" t="s">
-        <v>840</v>
+        <v>835</v>
       </c>
       <c r="B53" s="11" t="s">
         <v>737</v>
       </c>
       <c r="C53" s="11" t="s">
-        <v>841</v>
+        <v>836</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.35">
@@ -15471,13 +15354,13 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A55" s="11" t="s">
-        <v>878</v>
+        <v>865</v>
       </c>
       <c r="B55" s="11" t="s">
         <v>737</v>
       </c>
       <c r="C55" s="11" t="s">
-        <v>879</v>
+        <v>866</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.35">
@@ -15485,109 +15368,90 @@
         <v>755</v>
       </c>
       <c r="B56" s="11" t="s">
-        <v>1003</v>
+        <v>982</v>
       </c>
       <c r="C56" s="8" t="s">
-        <v>1004</v>
+        <v>983</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A57" s="11" t="s">
-        <v>133</v>
-      </c>
-      <c r="B57" s="11" t="s">
-        <v>889</v>
-      </c>
-      <c r="C57" s="47" t="s">
-        <v>890</v>
-      </c>
+      <c r="C57" s="47"/>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A58" s="11" t="s">
-        <v>837</v>
+        <v>832</v>
       </c>
       <c r="B58" s="11" t="s">
-        <v>838</v>
+        <v>833</v>
       </c>
       <c r="C58" s="11" t="s">
-        <v>839</v>
+        <v>834</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A59" s="11" t="s">
+        <v>815</v>
+      </c>
+      <c r="B59" s="11" t="s">
+        <v>816</v>
+      </c>
+      <c r="C59" s="11" t="s">
         <v>817</v>
-      </c>
-      <c r="B59" s="11" t="s">
-        <v>818</v>
-      </c>
-      <c r="C59" s="11" t="s">
-        <v>819</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A60" s="11" t="s">
-        <v>873</v>
-      </c>
-      <c r="B60" s="11" t="s">
-        <v>874</v>
-      </c>
-      <c r="C60" s="11" t="s">
-        <v>875</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A61" s="11" t="s">
+        <v>796</v>
+      </c>
+      <c r="B61" s="11" t="s">
+        <v>797</v>
+      </c>
+      <c r="C61" s="11" t="s">
         <v>798</v>
-      </c>
-      <c r="B61" s="11" t="s">
-        <v>799</v>
-      </c>
-      <c r="C61" s="11" t="s">
-        <v>800</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A62" s="11" t="s">
-        <v>857</v>
+        <v>849</v>
       </c>
       <c r="B62" s="11" t="s">
-        <v>858</v>
+        <v>850</v>
       </c>
       <c r="C62" s="11" t="s">
-        <v>859</v>
+        <v>851</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A63" s="11" t="s">
-        <v>1000</v>
+        <v>979</v>
       </c>
       <c r="B63" s="11" t="s">
-        <v>1001</v>
+        <v>980</v>
       </c>
       <c r="C63" s="19" t="s">
-        <v>1002</v>
+        <v>981</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A64" s="11" t="s">
+        <v>785</v>
+      </c>
+      <c r="B64" s="11" t="s">
+        <v>786</v>
+      </c>
+      <c r="C64" s="11" t="s">
         <v>787</v>
-      </c>
-      <c r="B64" s="11" t="s">
-        <v>788</v>
-      </c>
-      <c r="C64" s="11" t="s">
-        <v>789</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A65" s="11" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
       <c r="B65" s="11" t="s">
-        <v>788</v>
+        <v>786</v>
       </c>
       <c r="C65" s="11" t="s">
-        <v>791</v>
+        <v>789</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.35">
@@ -15595,21 +15459,10 @@
         <v>728</v>
       </c>
       <c r="B66" s="11" t="s">
-        <v>788</v>
+        <v>786</v>
       </c>
       <c r="C66" s="11" t="s">
-        <v>822</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A67" s="11" t="s">
-        <v>854</v>
-      </c>
-      <c r="B67" s="11" t="s">
-        <v>855</v>
-      </c>
-      <c r="C67" s="11" t="s">
-        <v>856</v>
+        <v>820</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.35">
@@ -15625,18 +15478,18 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A69" s="11" t="s">
+        <v>821</v>
+      </c>
+      <c r="B69" s="11" t="s">
+        <v>822</v>
+      </c>
+      <c r="C69" s="11" t="s">
         <v>823</v>
-      </c>
-      <c r="B69" s="11" t="s">
-        <v>824</v>
-      </c>
-      <c r="C69" s="11" t="s">
-        <v>825</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A70" s="11" t="s">
-        <v>1078</v>
+        <v>1057</v>
       </c>
       <c r="B70" s="11" t="s">
         <v>741</v>
@@ -15647,57 +15500,57 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A71" s="11" t="s">
-        <v>1063</v>
+        <v>1042</v>
       </c>
       <c r="B71" s="11" t="s">
-        <v>1068</v>
+        <v>1047</v>
       </c>
       <c r="C71" s="11" t="s">
-        <v>1067</v>
+        <v>1046</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A72" s="11" t="s">
-        <v>1069</v>
+        <v>1048</v>
       </c>
       <c r="B72" s="11" t="s">
-        <v>1001</v>
+        <v>980</v>
       </c>
       <c r="C72" s="11" t="s">
-        <v>1070</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A73" s="11" t="s">
-        <v>1064</v>
+        <v>1043</v>
       </c>
       <c r="B73" s="11" t="s">
-        <v>1071</v>
+        <v>1050</v>
       </c>
       <c r="C73" s="11" t="s">
-        <v>1072</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A74" s="11" t="s">
-        <v>1066</v>
+        <v>1045</v>
       </c>
       <c r="B74" s="11" t="s">
-        <v>1079</v>
+        <v>1058</v>
       </c>
       <c r="C74" s="11" t="s">
-        <v>1080</v>
+        <v>1059</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A75" s="11" t="s">
-        <v>1106</v>
+        <v>1085</v>
       </c>
       <c r="B75" s="11" t="s">
-        <v>1107</v>
+        <v>1086</v>
       </c>
       <c r="C75" s="11" t="s">
-        <v>1108</v>
+        <v>1087</v>
       </c>
     </row>
   </sheetData>
@@ -15717,7 +15570,7 @@
   <dimension ref="A1:E36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C2" sqref="C2:C27"/>
     </sheetView>
   </sheetViews>
@@ -15732,7 +15585,7 @@
   <sheetData>
     <row r="1" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="13" t="s">
-        <v>1074</v>
+        <v>1053</v>
       </c>
       <c r="B1" s="13" t="s">
         <v>622</v>
@@ -15746,30 +15599,30 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="11" t="s">
-        <v>902</v>
+        <v>881</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>903</v>
+        <v>882</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>904</v>
+        <v>883</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>895</v>
+        <v>874</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="11" t="s">
-        <v>892</v>
+        <v>871</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>893</v>
+        <v>872</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>894</v>
+        <v>873</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>895</v>
+        <v>874</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
@@ -15777,69 +15630,69 @@
         <v>748</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>897</v>
+        <v>876</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>898</v>
+        <v>877</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>1012</v>
+        <v>991</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="11" t="s">
-        <v>829</v>
+        <v>824</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>905</v>
+        <v>884</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>906</v>
+        <v>885</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>895</v>
+        <v>874</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="11" t="s">
-        <v>873</v>
+        <v>862</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>913</v>
+        <v>892</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>914</v>
+        <v>893</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>895</v>
+        <v>874</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="11" t="s">
-        <v>915</v>
+        <v>894</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>916</v>
+        <v>895</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>917</v>
+        <v>896</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>895</v>
+        <v>874</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="11" t="s">
-        <v>918</v>
+        <v>897</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>919</v>
+        <v>898</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>920</v>
+        <v>899</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>895</v>
+        <v>874</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
@@ -15847,55 +15700,55 @@
         <v>48</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>921</v>
+        <v>900</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>922</v>
+        <v>901</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>895</v>
+        <v>874</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="11" t="s">
-        <v>923</v>
+        <v>902</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>924</v>
+        <v>903</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>925</v>
+        <v>904</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>895</v>
+        <v>874</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="11" t="s">
-        <v>926</v>
+        <v>905</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>927</v>
+        <v>906</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>928</v>
+        <v>907</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>895</v>
+        <v>874</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="11" t="s">
-        <v>929</v>
+        <v>908</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>930</v>
+        <v>909</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>931</v>
+        <v>910</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>895</v>
+        <v>874</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
@@ -15903,41 +15756,41 @@
         <v>755</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>932</v>
+        <v>911</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>933</v>
+        <v>912</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>1011</v>
+        <v>990</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="11" t="s">
-        <v>934</v>
+        <v>913</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>932</v>
+        <v>911</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>935</v>
+        <v>914</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>1011</v>
+        <v>990</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="11" t="s">
-        <v>936</v>
+        <v>915</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>937</v>
+        <v>916</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>938</v>
+        <v>917</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>1010</v>
+        <v>989</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
@@ -15945,111 +15798,111 @@
         <v>128</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>939</v>
+        <v>918</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>940</v>
+        <v>919</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>895</v>
+        <v>874</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="11" t="s">
-        <v>941</v>
+        <v>920</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>942</v>
+        <v>921</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>943</v>
+        <v>922</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>895</v>
+        <v>874</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" s="11" t="s">
-        <v>907</v>
+        <v>886</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>908</v>
+        <v>887</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>909</v>
+        <v>888</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>895</v>
+        <v>874</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" s="11" t="s">
-        <v>944</v>
+        <v>923</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>945</v>
+        <v>924</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>946</v>
+        <v>925</v>
       </c>
       <c r="D19" s="11" t="s">
-        <v>895</v>
+        <v>874</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" s="11" t="s">
-        <v>947</v>
+        <v>926</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>948</v>
+        <v>927</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>949</v>
+        <v>928</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>895</v>
+        <v>874</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" s="11" t="s">
-        <v>950</v>
+        <v>929</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>951</v>
+        <v>930</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>952</v>
+        <v>931</v>
       </c>
       <c r="D21" s="11" t="s">
-        <v>895</v>
+        <v>874</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" s="11" t="s">
-        <v>1045</v>
+        <v>1024</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>1046</v>
+        <v>1025</v>
       </c>
       <c r="C22" s="38" t="s">
         <v>463</v>
       </c>
       <c r="D22" s="11" t="s">
-        <v>895</v>
+        <v>874</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" s="11" t="s">
-        <v>953</v>
+        <v>932</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>954</v>
+        <v>933</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>955</v>
+        <v>934</v>
       </c>
       <c r="D23" s="11" t="s">
-        <v>895</v>
+        <v>874</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
@@ -16057,60 +15910,60 @@
         <v>351</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>956</v>
+        <v>935</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>957</v>
+        <v>936</v>
       </c>
       <c r="D24" s="11" t="s">
-        <v>895</v>
+        <v>874</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" s="11" t="s">
-        <v>958</v>
+        <v>937</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>959</v>
+        <v>938</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>960</v>
+        <v>939</v>
       </c>
       <c r="D25" s="11" t="s">
-        <v>895</v>
+        <v>874</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" s="11" t="s">
-        <v>964</v>
+        <v>943</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>965</v>
+        <v>944</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>966</v>
+        <v>945</v>
       </c>
       <c r="D26" s="11" t="s">
-        <v>895</v>
+        <v>874</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" s="11" t="s">
-        <v>967</v>
+        <v>946</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>968</v>
+        <v>947</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>969</v>
+        <v>948</v>
       </c>
       <c r="D27" s="11" t="s">
-        <v>895</v>
+        <v>874</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" s="13" t="s">
-        <v>891</v>
+        <v>870</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
@@ -16118,55 +15971,55 @@
         <v>651</v>
       </c>
       <c r="B33" s="11" t="s">
-        <v>809</v>
+        <v>807</v>
       </c>
       <c r="D33" s="11" t="s">
-        <v>1013</v>
+        <v>992</v>
       </c>
       <c r="E33" s="11" t="s">
-        <v>896</v>
+        <v>875</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" s="11" t="s">
-        <v>899</v>
+        <v>878</v>
       </c>
       <c r="B34" s="11" t="s">
-        <v>900</v>
+        <v>879</v>
       </c>
       <c r="D34" s="11" t="s">
-        <v>1013</v>
+        <v>992</v>
       </c>
       <c r="E34" s="11" t="s">
-        <v>901</v>
+        <v>880</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" s="11" t="s">
-        <v>910</v>
+        <v>889</v>
       </c>
       <c r="B35" s="11" t="s">
-        <v>911</v>
+        <v>890</v>
       </c>
       <c r="D35" s="11" t="s">
-        <v>1013</v>
+        <v>992</v>
       </c>
       <c r="E35" s="11" t="s">
-        <v>912</v>
+        <v>891</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" s="11" t="s">
-        <v>961</v>
+        <v>940</v>
       </c>
       <c r="B36" s="11" t="s">
-        <v>962</v>
+        <v>941</v>
       </c>
       <c r="D36" s="11" t="s">
-        <v>1013</v>
+        <v>992</v>
       </c>
       <c r="E36" s="11" t="s">
-        <v>963</v>
+        <v>942</v>
       </c>
     </row>
   </sheetData>
@@ -16202,7 +16055,7 @@
   <sheetData>
     <row r="1" spans="1:4" s="45" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="45" t="s">
-        <v>1074</v>
+        <v>1053</v>
       </c>
       <c r="B1" s="45" t="s">
         <v>622</v>
@@ -16219,18 +16072,18 @@
         <v>10</v>
       </c>
       <c r="D2" s="44" t="s">
-        <v>987</v>
+        <v>966</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="44" t="s">
-        <v>978</v>
+        <v>957</v>
       </c>
       <c r="B3" s="44" t="s">
-        <v>979</v>
+        <v>958</v>
       </c>
       <c r="C3" s="44" t="s">
-        <v>980</v>
+        <v>959</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -16238,43 +16091,43 @@
         <v>629</v>
       </c>
       <c r="B4" s="44" t="s">
-        <v>988</v>
+        <v>967</v>
       </c>
       <c r="C4" s="44" t="s">
-        <v>989</v>
+        <v>968</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="44" t="s">
-        <v>981</v>
+        <v>960</v>
       </c>
       <c r="B5" s="44" t="s">
         <v>638</v>
       </c>
       <c r="C5" s="44" t="s">
-        <v>982</v>
+        <v>961</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="44" t="s">
-        <v>899</v>
+        <v>878</v>
       </c>
       <c r="B6" s="44" t="s">
-        <v>972</v>
+        <v>951</v>
       </c>
       <c r="C6" s="44" t="s">
-        <v>973</v>
+        <v>952</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="44" t="s">
-        <v>815</v>
+        <v>813</v>
       </c>
       <c r="B7" s="44" t="s">
-        <v>970</v>
+        <v>949</v>
       </c>
       <c r="C7" s="44" t="s">
-        <v>971</v>
+        <v>950</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -16285,40 +16138,40 @@
         <v>129</v>
       </c>
       <c r="D8" s="44" t="s">
-        <v>977</v>
+        <v>956</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="44" t="s">
-        <v>974</v>
+        <v>953</v>
       </c>
       <c r="B9" s="44" t="s">
-        <v>975</v>
+        <v>954</v>
       </c>
       <c r="C9" s="44" t="s">
-        <v>976</v>
+        <v>955</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="44" t="s">
-        <v>974</v>
+        <v>953</v>
       </c>
       <c r="B10" s="44" t="s">
-        <v>983</v>
+        <v>962</v>
       </c>
       <c r="C10" s="44" t="s">
-        <v>984</v>
+        <v>963</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="44" t="s">
-        <v>992</v>
+        <v>971</v>
       </c>
       <c r="B11" s="44" t="s">
-        <v>993</v>
+        <v>972</v>
       </c>
       <c r="C11" s="44" t="s">
-        <v>994</v>
+        <v>973</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -16326,15 +16179,15 @@
         <v>647</v>
       </c>
       <c r="B12" s="44" t="s">
-        <v>985</v>
+        <v>964</v>
       </c>
       <c r="C12" s="44" t="s">
-        <v>986</v>
+        <v>965</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="44" t="s">
-        <v>1044</v>
+        <v>1023</v>
       </c>
       <c r="B13" s="44" t="s">
         <v>386</v>
@@ -16342,7 +16195,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="45" t="s">
-        <v>891</v>
+        <v>870</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
@@ -16350,21 +16203,21 @@
         <v>637</v>
       </c>
       <c r="B20" s="44" t="s">
-        <v>990</v>
+        <v>969</v>
       </c>
       <c r="D20" s="44" t="s">
-        <v>991</v>
+        <v>970</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="44" t="s">
-        <v>992</v>
+        <v>971</v>
       </c>
       <c r="B21" s="44" t="s">
-        <v>993</v>
+        <v>972</v>
       </c>
       <c r="D21" s="44" t="s">
-        <v>994</v>
+        <v>973</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
@@ -16372,21 +16225,21 @@
         <v>755</v>
       </c>
       <c r="B22" s="44" t="s">
-        <v>995</v>
+        <v>974</v>
       </c>
       <c r="D22" s="44" t="s">
-        <v>996</v>
+        <v>975</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="44" t="s">
-        <v>997</v>
+        <v>976</v>
       </c>
       <c r="B23" s="44" t="s">
-        <v>998</v>
+        <v>977</v>
       </c>
       <c r="D23" s="44" t="s">
-        <v>999</v>
+        <v>978</v>
       </c>
     </row>
   </sheetData>
@@ -16420,7 +16273,7 @@
   <sheetData>
     <row r="1" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="13" t="s">
-        <v>1074</v>
+        <v>1053</v>
       </c>
       <c r="B1" s="13" t="s">
         <v>1</v>
@@ -16429,10 +16282,10 @@
         <v>5</v>
       </c>
       <c r="D1" s="13" t="s">
-        <v>1020</v>
+        <v>999</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>1021</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
@@ -16440,7 +16293,7 @@
         <v>30</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>1081</v>
+        <v>1060</v>
       </c>
       <c r="F2" s="11" t="s">
         <v>34</v>
@@ -16448,16 +16301,16 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="11" t="s">
-        <v>1087</v>
+        <v>1066</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>1088</v>
+        <v>1067</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>1093</v>
+        <v>1072</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>1065</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
@@ -16465,27 +16318,27 @@
         <v>9</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>1083</v>
+        <v>1062</v>
       </c>
       <c r="C4" s="38" t="s">
-        <v>1105</v>
+        <v>1084</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>1085</v>
+        <v>1064</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>1089</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="11" t="s">
-        <v>1084</v>
+        <v>1063</v>
       </c>
       <c r="B5" s="11" t="s">
         <v>658</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>1086</v>
+        <v>1065</v>
       </c>
       <c r="D5" s="11" t="s">
         <v>161</v>
@@ -16496,13 +16349,13 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="11" t="s">
-        <v>1090</v>
+        <v>1069</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>1091</v>
+        <v>1070</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>1092</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Add landmark plaque details for Julia Morgan Building
</commit_message>
<xml_diff>
--- a/3-1-heritage/0-heritage-happenings/2025/04-april-hh/resident-directory/2025-04-heritage-resident-directory.xlsx
+++ b/3-1-heritage/0-heritage-happenings/2025/04-april-hh/resident-directory/2025-04-heritage-resident-directory.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4348e1419f457eb2/Documents/GitHub/theo-armour-agenda/3-1-heritage/0-heritage-happenings/2025/04-april-hh/resident-directory/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="970" documentId="8_{47523533-A004-48EF-BEEC-0FA3DE3C4717}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{48DF991E-94E1-424A-8471-F753BE537874}"/>
+  <xr:revisionPtr revIDLastSave="977" documentId="8_{47523533-A004-48EF-BEEC-0FA3DE3C4717}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1D5E067C-32C3-4A3F-B833-6A27FE94C34B}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="754" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="754" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Residents" sheetId="1" r:id="rId1"/>
@@ -2721,9 +2721,6 @@
     <t>Abad</t>
   </si>
   <si>
-    <t>&lt;gabad@heritagesf.org&gt;</t>
-  </si>
-  <si>
     <t>Camarota</t>
   </si>
   <si>
@@ -2733,12 +2730,6 @@
     <t>Alvin</t>
   </si>
   <si>
-    <t>Lachan</t>
-  </si>
-  <si>
-    <t>&lt;rlachan@heritagesf.org&gt;</t>
-  </si>
-  <si>
     <t>Irving</t>
   </si>
   <si>
@@ -3562,6 +3553,15 @@
   </si>
   <si>
     <t>jennifer@arthurassociates.net</t>
+  </si>
+  <si>
+    <t>vabad@heritagesf.org</t>
+  </si>
+  <si>
+    <t>Lochan</t>
+  </si>
+  <si>
+    <t>&lt;rlochan@heritagesf.org&gt;</t>
   </si>
 </sst>
 </file>
@@ -4215,6 +4215,10 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
@@ -4439,7 +4443,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="17" t="s">
-        <v>1053</v>
+        <v>1050</v>
       </c>
       <c r="B1" s="17" t="s">
         <v>1</v>
@@ -4552,17 +4556,17 @@
         <v>778</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>1161</v>
+        <v>1158</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1" t="s">
         <v>38</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>1162</v>
+        <v>1159</v>
       </c>
       <c r="F5" s="40" t="s">
-        <v>1163</v>
+        <v>1160</v>
       </c>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
@@ -4972,10 +4976,10 @@
     </row>
     <row r="22" spans="1:9" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A22" s="17" t="s">
-        <v>993</v>
+        <v>990</v>
       </c>
       <c r="B22" s="17" t="s">
-        <v>994</v>
+        <v>991</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>19</v>
@@ -4984,10 +4988,10 @@
         <v>38</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>995</v>
+        <v>992</v>
       </c>
       <c r="F22" s="40" t="s">
-        <v>997</v>
+        <v>994</v>
       </c>
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
@@ -5187,7 +5191,7 @@
         <v>19</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>1082</v>
+        <v>1079</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>163</v>
@@ -5507,7 +5511,7 @@
         <v>19</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>1073</v>
+        <v>1070</v>
       </c>
       <c r="E43" s="1" t="s">
         <v>231</v>
@@ -5524,7 +5528,7 @@
     </row>
     <row r="44" spans="1:9" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A44" s="17" t="s">
-        <v>1028</v>
+        <v>1025</v>
       </c>
       <c r="B44" s="17" t="s">
         <v>233</v>
@@ -5738,22 +5742,22 @@
     </row>
     <row r="53" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="17" t="s">
+        <v>1071</v>
+      </c>
+      <c r="B53" s="17" t="s">
+        <v>1072</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>1073</v>
+      </c>
+      <c r="E53" s="1" t="s">
         <v>1074</v>
       </c>
-      <c r="B53" s="17" t="s">
+      <c r="F53" s="39" t="s">
         <v>1075</v>
       </c>
-      <c r="D53" s="1" t="s">
+      <c r="I53" s="53" t="s">
         <v>1076</v>
-      </c>
-      <c r="E53" s="1" t="s">
-        <v>1077</v>
-      </c>
-      <c r="F53" s="39" t="s">
-        <v>1078</v>
-      </c>
-      <c r="I53" s="53" t="s">
-        <v>1079</v>
       </c>
     </row>
     <row r="54" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -5761,19 +5765,19 @@
         <v>843</v>
       </c>
       <c r="B54" s="17" t="s">
-        <v>1075</v>
+        <v>1072</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>1076</v>
+        <v>1073</v>
       </c>
       <c r="E54" s="1" t="s">
+        <v>1077</v>
+      </c>
+      <c r="F54" s="40" t="s">
         <v>1080</v>
       </c>
-      <c r="F54" s="40" t="s">
-        <v>1083</v>
-      </c>
       <c r="I54" s="53" t="s">
-        <v>1081</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="55" spans="1:9" ht="13.5" x14ac:dyDescent="0.3">
@@ -5822,7 +5826,7 @@
         <v>288</v>
       </c>
       <c r="F56" s="49" t="s">
-        <v>1052</v>
+        <v>1049</v>
       </c>
       <c r="G56" s="1"/>
       <c r="H56" s="1"/>
@@ -9162,7 +9166,7 @@
     </row>
     <row r="3" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>1054</v>
+        <v>1051</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>17</v>
@@ -11370,7 +11374,7 @@
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A79" s="11" t="s">
-        <v>996</v>
+        <v>993</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.35">
@@ -11389,7 +11393,7 @@
     </row>
     <row r="82" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A82" s="52" t="s">
-        <v>1061</v>
+        <v>1058</v>
       </c>
       <c r="B82" s="52"/>
       <c r="C82" s="52"/>
@@ -12628,7 +12632,7 @@
   <sheetData>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>1117</v>
+        <v>1114</v>
       </c>
       <c r="B2" t="s">
         <v>174</v>
@@ -12636,7 +12640,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>1121</v>
+        <v>1118</v>
       </c>
       <c r="B3" t="s">
         <v>174</v>
@@ -12644,7 +12648,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>1155</v>
+        <v>1152</v>
       </c>
       <c r="B4" t="s">
         <v>174</v>
@@ -12652,7 +12656,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>1160</v>
+        <v>1157</v>
       </c>
       <c r="B5" t="s">
         <v>174</v>
@@ -12660,7 +12664,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>1103</v>
+        <v>1100</v>
       </c>
       <c r="B6" t="s">
         <v>110</v>
@@ -12668,7 +12672,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>1114</v>
+        <v>1111</v>
       </c>
       <c r="B7" t="s">
         <v>160</v>
@@ -12676,7 +12680,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>1108</v>
+        <v>1105</v>
       </c>
       <c r="B8" t="s">
         <v>132</v>
@@ -12684,7 +12688,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>1143</v>
+        <v>1140</v>
       </c>
       <c r="B9" t="s">
         <v>301</v>
@@ -12692,7 +12696,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>1126</v>
+        <v>1123</v>
       </c>
       <c r="B10" t="s">
         <v>222</v>
@@ -12700,7 +12704,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>1154</v>
+        <v>1151</v>
       </c>
       <c r="B11" t="s">
         <v>222</v>
@@ -12708,7 +12712,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>1090</v>
+        <v>1087</v>
       </c>
       <c r="B12" t="s">
         <v>35</v>
@@ -12716,15 +12720,15 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>1138</v>
+        <v>1135</v>
       </c>
       <c r="B13" t="s">
-        <v>1079</v>
+        <v>1076</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>1106</v>
+        <v>1103</v>
       </c>
       <c r="B14" t="s">
         <v>127</v>
@@ -12732,7 +12736,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>1151</v>
+        <v>1148</v>
       </c>
       <c r="B15" t="s">
         <v>127</v>
@@ -12740,7 +12744,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>1107</v>
+        <v>1104</v>
       </c>
       <c r="B16" t="s">
         <v>342</v>
@@ -12748,7 +12752,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>1150</v>
+        <v>1147</v>
       </c>
       <c r="B17" t="s">
         <v>342</v>
@@ -12756,7 +12760,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>1127</v>
+        <v>1124</v>
       </c>
       <c r="B18" t="s">
         <v>228</v>
@@ -12764,7 +12768,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>1123</v>
+        <v>1120</v>
       </c>
       <c r="B19" t="s">
         <v>208</v>
@@ -12772,7 +12776,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>1104</v>
+        <v>1101</v>
       </c>
       <c r="B20" t="s">
         <v>116</v>
@@ -12780,15 +12784,15 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>1139</v>
+        <v>1136</v>
       </c>
       <c r="B21" t="s">
-        <v>1081</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>1142</v>
+        <v>1139</v>
       </c>
       <c r="B22" t="s">
         <v>295</v>
@@ -12796,7 +12800,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>1100</v>
+        <v>1097</v>
       </c>
       <c r="B23" t="s">
         <v>94</v>
@@ -12804,7 +12808,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>1095</v>
+        <v>1092</v>
       </c>
       <c r="B24" t="s">
         <v>62</v>
@@ -12812,7 +12816,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>1145</v>
+        <v>1142</v>
       </c>
       <c r="B25" t="s">
         <v>312</v>
@@ -12820,7 +12824,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>1153</v>
+        <v>1150</v>
       </c>
       <c r="B26" t="s">
         <v>355</v>
@@ -12828,7 +12832,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>1146</v>
+        <v>1143</v>
       </c>
       <c r="B27" t="s">
         <v>317</v>
@@ -12836,7 +12840,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>1147</v>
+        <v>1144</v>
       </c>
       <c r="B28" t="s">
         <v>327</v>
@@ -12844,7 +12848,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>1141</v>
+        <v>1138</v>
       </c>
       <c r="B29" t="s">
         <v>289</v>
@@ -12852,7 +12856,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>1116</v>
+        <v>1113</v>
       </c>
       <c r="B30" t="s">
         <v>170</v>
@@ -12860,7 +12864,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>1119</v>
+        <v>1116</v>
       </c>
       <c r="B31" t="s">
         <v>186</v>
@@ -12868,7 +12872,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>1156</v>
+        <v>1153</v>
       </c>
       <c r="B32" t="s">
         <v>369</v>
@@ -12876,7 +12880,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>1118</v>
+        <v>1115</v>
       </c>
       <c r="B33" t="s">
         <v>180</v>
@@ -12884,7 +12888,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>1098</v>
+        <v>1095</v>
       </c>
       <c r="B34" t="s">
         <v>84</v>
@@ -12892,7 +12896,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>1102</v>
+        <v>1099</v>
       </c>
       <c r="B35" t="s">
         <v>104</v>
@@ -12900,7 +12904,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>1149</v>
+        <v>1146</v>
       </c>
       <c r="B36" t="s">
         <v>336</v>
@@ -12908,7 +12912,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>1109</v>
+        <v>1106</v>
       </c>
       <c r="B37" t="s">
         <v>135</v>
@@ -12916,7 +12920,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>1111</v>
+        <v>1108</v>
       </c>
       <c r="B38" t="s">
         <v>147</v>
@@ -12924,7 +12928,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>1128</v>
+        <v>1125</v>
       </c>
       <c r="B39" t="s">
         <v>147</v>
@@ -12932,7 +12936,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>1158</v>
+        <v>1155</v>
       </c>
       <c r="B40" t="s">
         <v>381</v>
@@ -12940,7 +12944,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>1092</v>
+        <v>1089</v>
       </c>
       <c r="B41" t="s">
         <v>47</v>
@@ -12948,7 +12952,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>1135</v>
+        <v>1132</v>
       </c>
       <c r="B42" t="s">
         <v>268</v>
@@ -12956,7 +12960,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>1125</v>
+        <v>1122</v>
       </c>
       <c r="B43" t="s">
         <v>219</v>
@@ -12964,7 +12968,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>1124</v>
+        <v>1121</v>
       </c>
       <c r="B44" t="s">
         <v>213</v>
@@ -12972,7 +12976,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>1096</v>
+        <v>1093</v>
       </c>
       <c r="B45" t="s">
         <v>68</v>
@@ -12980,7 +12984,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>1130</v>
+        <v>1127</v>
       </c>
       <c r="B46" t="s">
         <v>68</v>
@@ -12988,7 +12992,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>1148</v>
+        <v>1145</v>
       </c>
       <c r="B47" t="s">
         <v>332</v>
@@ -12996,7 +13000,7 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>1132</v>
+        <v>1129</v>
       </c>
       <c r="B48" t="s">
         <v>252</v>
@@ -13004,7 +13008,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>1088</v>
+        <v>1085</v>
       </c>
       <c r="B49" t="s">
         <v>16</v>
@@ -13012,7 +13016,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>1136</v>
+        <v>1133</v>
       </c>
       <c r="B50" t="s">
         <v>273</v>
@@ -13020,7 +13024,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>1097</v>
+        <v>1094</v>
       </c>
       <c r="B51" t="s">
         <v>79</v>
@@ -13028,7 +13032,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>1089</v>
+        <v>1086</v>
       </c>
       <c r="B52" t="s">
         <v>29</v>
@@ -13036,7 +13040,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>1157</v>
+        <v>1154</v>
       </c>
       <c r="B53" t="s">
         <v>374</v>
@@ -13044,7 +13048,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>1120</v>
+        <v>1117</v>
       </c>
       <c r="B54" t="s">
         <v>192</v>
@@ -13052,7 +13056,7 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>1093</v>
+        <v>1090</v>
       </c>
       <c r="B55" t="s">
         <v>54</v>
@@ -13060,7 +13064,7 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>1140</v>
+        <v>1137</v>
       </c>
       <c r="B56" t="s">
         <v>54</v>
@@ -13068,7 +13072,7 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>1110</v>
+        <v>1107</v>
       </c>
       <c r="B57" t="s">
         <v>141</v>
@@ -13076,7 +13080,7 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>1122</v>
+        <v>1119</v>
       </c>
       <c r="B58" t="s">
         <v>203</v>
@@ -13084,7 +13088,7 @@
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>1094</v>
+        <v>1091</v>
       </c>
       <c r="B59" t="s">
         <v>56</v>
@@ -13092,7 +13096,7 @@
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>1137</v>
+        <v>1134</v>
       </c>
       <c r="B60" t="s">
         <v>277</v>
@@ -13100,7 +13104,7 @@
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>1112</v>
+        <v>1109</v>
       </c>
       <c r="B61" t="s">
         <v>152</v>
@@ -13108,7 +13112,7 @@
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>1113</v>
+        <v>1110</v>
       </c>
       <c r="B62" t="s">
         <v>154</v>
@@ -13116,7 +13120,7 @@
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>1105</v>
+        <v>1102</v>
       </c>
       <c r="B63" t="s">
         <v>122</v>
@@ -13124,7 +13128,7 @@
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>1091</v>
+        <v>1088</v>
       </c>
       <c r="B64" t="s">
         <v>41</v>
@@ -13132,7 +13136,7 @@
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>1159</v>
+        <v>1156</v>
       </c>
       <c r="B65" t="s">
         <v>385</v>
@@ -13140,7 +13144,7 @@
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>1144</v>
+        <v>1141</v>
       </c>
       <c r="B66" t="s">
         <v>306</v>
@@ -13148,7 +13152,7 @@
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>1133</v>
+        <v>1130</v>
       </c>
       <c r="B67" t="s">
         <v>257</v>
@@ -13156,7 +13160,7 @@
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>1152</v>
+        <v>1149</v>
       </c>
       <c r="B68" t="s">
         <v>257</v>
@@ -13164,7 +13168,7 @@
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>1115</v>
+        <v>1112</v>
       </c>
       <c r="B69" t="s">
         <v>165</v>
@@ -13172,7 +13176,7 @@
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>1134</v>
+        <v>1131</v>
       </c>
       <c r="B70" t="s">
         <v>165</v>
@@ -13180,7 +13184,7 @@
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>1129</v>
+        <v>1126</v>
       </c>
       <c r="B71" t="s">
         <v>237</v>
@@ -13188,7 +13192,7 @@
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>1101</v>
+        <v>1098</v>
       </c>
       <c r="B72" t="s">
         <v>99</v>
@@ -13196,7 +13200,7 @@
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>1099</v>
+        <v>1096</v>
       </c>
       <c r="B73" t="s">
         <v>90</v>
@@ -13204,7 +13208,7 @@
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>1131</v>
+        <v>1128</v>
       </c>
       <c r="B74" t="s">
         <v>247</v>
@@ -13224,7 +13228,7 @@
   <dimension ref="A1:E100"/>
   <sheetViews>
     <sheetView showWhiteSpace="0" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C2" sqref="C2:C62"/>
     </sheetView>
   </sheetViews>
@@ -13240,19 +13244,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="27" t="s">
-        <v>1053</v>
+        <v>1050</v>
       </c>
       <c r="B1" s="27" t="s">
-        <v>998</v>
+        <v>995</v>
       </c>
       <c r="C1" s="20" t="s">
         <v>5</v>
       </c>
       <c r="D1" s="27" t="s">
-        <v>999</v>
+        <v>996</v>
       </c>
       <c r="E1" s="27" t="s">
-        <v>1000</v>
+        <v>997</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
@@ -13277,13 +13281,13 @@
         <v>748</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>1034</v>
+        <v>1031</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>1033</v>
+        <v>1030</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>1032</v>
+        <v>1029</v>
       </c>
       <c r="E3" s="11" t="s">
         <v>25</v>
@@ -13317,10 +13321,10 @@
         <v>639</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>1007</v>
+        <v>1004</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>1008</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
@@ -13379,7 +13383,7 @@
         <v>645</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>1019</v>
+        <v>1016</v>
       </c>
       <c r="C9" s="19" t="s">
         <v>646</v>
@@ -13396,7 +13400,7 @@
         <v>647</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>1001</v>
+        <v>998</v>
       </c>
       <c r="C10" s="19" t="s">
         <v>648</v>
@@ -13436,7 +13440,7 @@
         <v>652</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>1011</v>
+        <v>1008</v>
       </c>
       <c r="E12" s="11" t="s">
         <v>143</v>
@@ -13512,7 +13516,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="11" t="s">
-        <v>1012</v>
+        <v>1009</v>
       </c>
       <c r="B17" s="11" t="s">
         <v>166</v>
@@ -13617,16 +13621,16 @@
         <v>661</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>1002</v>
+        <v>999</v>
       </c>
       <c r="C23" s="19" t="s">
-        <v>1003</v>
+        <v>1000</v>
       </c>
       <c r="D23" s="11" t="s">
         <v>171</v>
       </c>
       <c r="E23" s="11" t="s">
-        <v>1004</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
@@ -13634,7 +13638,7 @@
         <v>662</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>1002</v>
+        <v>999</v>
       </c>
       <c r="C24" s="19" t="s">
         <v>663</v>
@@ -13643,18 +13647,18 @@
         <v>171</v>
       </c>
       <c r="E24" s="11" t="s">
-        <v>1004</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="38" t="s">
-        <v>1029</v>
+        <v>1026</v>
       </c>
       <c r="B25" s="38" t="s">
         <v>188</v>
       </c>
       <c r="C25" s="38" t="s">
-        <v>1030</v>
+        <v>1027</v>
       </c>
       <c r="D25" s="19" t="s">
         <v>187</v>
@@ -13671,7 +13675,7 @@
         <v>188</v>
       </c>
       <c r="C26" s="38" t="s">
-        <v>1031</v>
+        <v>1028</v>
       </c>
       <c r="D26" s="19" t="s">
         <v>187</v>
@@ -13685,7 +13689,7 @@
         <v>664</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>1016</v>
+        <v>1013</v>
       </c>
       <c r="C27" s="19" t="s">
         <v>665</v>
@@ -13756,7 +13760,7 @@
         <v>230</v>
       </c>
       <c r="C31" s="19" t="s">
-        <v>1013</v>
+        <v>1010</v>
       </c>
       <c r="D31" s="11" t="s">
         <v>229</v>
@@ -13767,16 +13771,16 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" s="11" t="s">
-        <v>1036</v>
+        <v>1033</v>
       </c>
       <c r="B32" s="11" t="s">
         <v>233</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>1035</v>
+        <v>1032</v>
       </c>
       <c r="D32" s="11" t="s">
-        <v>1028</v>
+        <v>1025</v>
       </c>
       <c r="E32" s="11" t="s">
         <v>233</v>
@@ -13784,13 +13788,13 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" s="11" t="s">
-        <v>1041</v>
+        <v>1038</v>
       </c>
       <c r="B33" s="11" t="s">
         <v>249</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>1040</v>
+        <v>1037</v>
       </c>
       <c r="D33" s="11" t="s">
         <v>248</v>
@@ -13835,13 +13839,13 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" s="11" t="s">
-        <v>1037</v>
+        <v>1034</v>
       </c>
       <c r="B36" s="11" t="s">
-        <v>1038</v>
+        <v>1035</v>
       </c>
       <c r="C36" s="11" t="s">
-        <v>1039</v>
+        <v>1036</v>
       </c>
       <c r="D36" s="11" t="s">
         <v>258</v>
@@ -13906,13 +13910,13 @@
         <v>684</v>
       </c>
       <c r="B40" s="11" t="s">
-        <v>1005</v>
+        <v>1002</v>
       </c>
       <c r="C40" s="19" t="s">
         <v>685</v>
       </c>
       <c r="D40" s="11" t="s">
-        <v>1006</v>
+        <v>1003</v>
       </c>
       <c r="E40" s="11" t="s">
         <v>270</v>
@@ -13929,7 +13933,7 @@
         <v>683</v>
       </c>
       <c r="D41" s="11" t="s">
-        <v>1006</v>
+        <v>1003</v>
       </c>
       <c r="E41" s="11" t="s">
         <v>270</v>
@@ -13946,7 +13950,7 @@
         <v>682</v>
       </c>
       <c r="D42" s="11" t="s">
-        <v>1006</v>
+        <v>1003</v>
       </c>
       <c r="E42" s="11" t="s">
         <v>270</v>
@@ -13957,13 +13961,13 @@
         <v>193</v>
       </c>
       <c r="B43" s="11" t="s">
-        <v>1015</v>
+        <v>1012</v>
       </c>
       <c r="C43" s="38" t="s">
-        <v>1055</v>
+        <v>1052</v>
       </c>
       <c r="D43" s="11" t="s">
-        <v>1006</v>
+        <v>1003</v>
       </c>
       <c r="E43" s="11" t="s">
         <v>270</v>
@@ -14014,7 +14018,7 @@
         <v>690</v>
       </c>
       <c r="D46" s="11" t="s">
-        <v>1020</v>
+        <v>1017</v>
       </c>
       <c r="E46" s="11" t="s">
         <v>283</v>
@@ -14031,7 +14035,7 @@
         <v>692</v>
       </c>
       <c r="D47" s="11" t="s">
-        <v>1020</v>
+        <v>1017</v>
       </c>
       <c r="E47" s="11" t="s">
         <v>283</v>
@@ -14042,13 +14046,13 @@
         <v>693</v>
       </c>
       <c r="B48" s="11" t="s">
-        <v>1021</v>
+        <v>1018</v>
       </c>
       <c r="C48" s="19" t="s">
         <v>694</v>
       </c>
       <c r="D48" s="11" t="s">
-        <v>1020</v>
+        <v>1017</v>
       </c>
       <c r="E48" s="11" t="s">
         <v>283</v>
@@ -14079,7 +14083,7 @@
         <v>297</v>
       </c>
       <c r="C50" s="38" t="s">
-        <v>1056</v>
+        <v>1053</v>
       </c>
       <c r="D50" s="11" t="s">
         <v>296</v>
@@ -14110,7 +14114,7 @@
         <v>701</v>
       </c>
       <c r="B52" s="11" t="s">
-        <v>1017</v>
+        <v>1014</v>
       </c>
       <c r="C52" s="19" t="s">
         <v>702</v>
@@ -14124,7 +14128,7 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A53" s="11" t="s">
-        <v>1022</v>
+        <v>1019</v>
       </c>
       <c r="B53" s="11" t="s">
         <v>314</v>
@@ -14178,7 +14182,7 @@
         <v>706</v>
       </c>
       <c r="B56" s="11" t="s">
-        <v>1014</v>
+        <v>1011</v>
       </c>
       <c r="C56" s="19" t="s">
         <v>707</v>
@@ -14195,7 +14199,7 @@
         <v>804</v>
       </c>
       <c r="B57" s="11" t="s">
-        <v>1018</v>
+        <v>1015</v>
       </c>
       <c r="C57" s="19" t="s">
         <v>705</v>
@@ -14249,10 +14253,10 @@
         <v>719</v>
       </c>
       <c r="C60" s="38" t="s">
-        <v>1009</v>
+        <v>1006</v>
       </c>
       <c r="D60" s="11" t="s">
-        <v>1010</v>
+        <v>1007</v>
       </c>
       <c r="E60" s="11" t="s">
         <v>376</v>
@@ -14269,7 +14273,7 @@
         <v>717</v>
       </c>
       <c r="D61" s="11" t="s">
-        <v>1010</v>
+        <v>1007</v>
       </c>
       <c r="E61" s="11" t="s">
         <v>376</v>
@@ -14286,7 +14290,7 @@
         <v>715</v>
       </c>
       <c r="D62" s="11" t="s">
-        <v>1010</v>
+        <v>1007</v>
       </c>
       <c r="E62" s="11" t="s">
         <v>376</v>
@@ -14681,7 +14685,7 @@
         <v>233</v>
       </c>
       <c r="B24" s="48" t="s">
-        <v>1028</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
@@ -14797,8 +14801,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CAA4147-474C-47CD-A0DD-4C67000E8368}">
   <dimension ref="A1:C75"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C13" sqref="A13:C13"/>
     </sheetView>
   </sheetViews>
@@ -14815,7 +14819,7 @@
   <sheetData>
     <row r="1" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="13" t="s">
-        <v>1053</v>
+        <v>1050</v>
       </c>
       <c r="B1" s="13" t="s">
         <v>622</v>
@@ -14881,7 +14885,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="8" t="s">
-        <v>1026</v>
+        <v>1023</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>31</v>
@@ -14914,7 +14918,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="11" t="s">
-        <v>1027</v>
+        <v>1024</v>
       </c>
       <c r="B10" s="11" t="s">
         <v>743</v>
@@ -15024,13 +15028,13 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="11" t="s">
-        <v>984</v>
+        <v>981</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>985</v>
+        <v>982</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>986</v>
+        <v>983</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
@@ -15225,10 +15229,10 @@
         <v>672</v>
       </c>
       <c r="B42" s="11" t="s">
-        <v>987</v>
+        <v>984</v>
       </c>
       <c r="C42" s="11" t="s">
-        <v>988</v>
+        <v>985</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.35">
@@ -15368,10 +15372,10 @@
         <v>755</v>
       </c>
       <c r="B56" s="11" t="s">
-        <v>982</v>
+        <v>979</v>
       </c>
       <c r="C56" s="8" t="s">
-        <v>983</v>
+        <v>980</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.35">
@@ -15423,13 +15427,13 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A63" s="11" t="s">
-        <v>979</v>
+        <v>976</v>
       </c>
       <c r="B63" s="11" t="s">
-        <v>980</v>
+        <v>977</v>
       </c>
       <c r="C63" s="19" t="s">
-        <v>981</v>
+        <v>978</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.35">
@@ -15489,7 +15493,7 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A70" s="11" t="s">
-        <v>1057</v>
+        <v>1054</v>
       </c>
       <c r="B70" s="11" t="s">
         <v>741</v>
@@ -15500,57 +15504,57 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A71" s="11" t="s">
-        <v>1042</v>
+        <v>1039</v>
       </c>
       <c r="B71" s="11" t="s">
-        <v>1047</v>
+        <v>1044</v>
       </c>
       <c r="C71" s="11" t="s">
-        <v>1046</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A72" s="11" t="s">
-        <v>1048</v>
+        <v>1045</v>
       </c>
       <c r="B72" s="11" t="s">
-        <v>980</v>
+        <v>977</v>
       </c>
       <c r="C72" s="11" t="s">
-        <v>1049</v>
+        <v>1046</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A73" s="11" t="s">
-        <v>1043</v>
+        <v>1040</v>
       </c>
       <c r="B73" s="11" t="s">
-        <v>1050</v>
+        <v>1047</v>
       </c>
       <c r="C73" s="11" t="s">
-        <v>1051</v>
+        <v>1048</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A74" s="11" t="s">
-        <v>1045</v>
+        <v>1042</v>
       </c>
       <c r="B74" s="11" t="s">
-        <v>1058</v>
+        <v>1055</v>
       </c>
       <c r="C74" s="11" t="s">
-        <v>1059</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A75" s="11" t="s">
-        <v>1085</v>
+        <v>1082</v>
       </c>
       <c r="B75" s="11" t="s">
-        <v>1086</v>
+        <v>1083</v>
       </c>
       <c r="C75" s="11" t="s">
-        <v>1087</v>
+        <v>1084</v>
       </c>
     </row>
   </sheetData>
@@ -15569,9 +15573,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{125B352A-F0BB-4FBB-AB9A-46907AE2C1C2}">
   <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2:C27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C27" sqref="C2:C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23046875" defaultRowHeight="17.5" x14ac:dyDescent="0.35"/>
@@ -15585,7 +15589,7 @@
   <sheetData>
     <row r="1" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="13" t="s">
-        <v>1053</v>
+        <v>1050</v>
       </c>
       <c r="B1" s="13" t="s">
         <v>622</v>
@@ -15604,8 +15608,8 @@
       <c r="B2" s="11" t="s">
         <v>882</v>
       </c>
-      <c r="C2" s="11" t="s">
-        <v>883</v>
+      <c r="C2" s="38" t="s">
+        <v>1161</v>
       </c>
       <c r="D2" s="11" t="s">
         <v>874</v>
@@ -15636,7 +15640,7 @@
         <v>877</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>991</v>
+        <v>988</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
@@ -15644,10 +15648,10 @@
         <v>824</v>
       </c>
       <c r="B5" s="11" t="s">
+        <v>883</v>
+      </c>
+      <c r="C5" s="11" t="s">
         <v>884</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>885</v>
       </c>
       <c r="D5" s="11" t="s">
         <v>874</v>
@@ -15658,10 +15662,10 @@
         <v>862</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>892</v>
+        <v>889</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>893</v>
+        <v>890</v>
       </c>
       <c r="D6" s="11" t="s">
         <v>874</v>
@@ -15669,13 +15673,13 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="11" t="s">
-        <v>894</v>
+        <v>891</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>895</v>
+        <v>892</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>896</v>
+        <v>893</v>
       </c>
       <c r="D7" s="11" t="s">
         <v>874</v>
@@ -15683,13 +15687,13 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="11" t="s">
-        <v>897</v>
+        <v>894</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>898</v>
+        <v>895</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>899</v>
+        <v>896</v>
       </c>
       <c r="D8" s="11" t="s">
         <v>874</v>
@@ -15700,10 +15704,10 @@
         <v>48</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>900</v>
+        <v>897</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>901</v>
+        <v>898</v>
       </c>
       <c r="D9" s="11" t="s">
         <v>874</v>
@@ -15711,13 +15715,13 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="11" t="s">
-        <v>902</v>
+        <v>899</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>903</v>
+        <v>900</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>904</v>
+        <v>901</v>
       </c>
       <c r="D10" s="11" t="s">
         <v>874</v>
@@ -15725,13 +15729,13 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="11" t="s">
-        <v>905</v>
+        <v>902</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>906</v>
+        <v>903</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>907</v>
+        <v>904</v>
       </c>
       <c r="D11" s="11" t="s">
         <v>874</v>
@@ -15739,13 +15743,13 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="11" t="s">
-        <v>908</v>
+        <v>905</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>909</v>
+        <v>906</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>910</v>
+        <v>907</v>
       </c>
       <c r="D12" s="11" t="s">
         <v>874</v>
@@ -15756,41 +15760,41 @@
         <v>755</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>911</v>
+        <v>908</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>912</v>
+        <v>909</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>990</v>
+        <v>987</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="11" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
       <c r="B14" s="11" t="s">
+        <v>908</v>
+      </c>
+      <c r="C14" s="11" t="s">
         <v>911</v>
       </c>
-      <c r="C14" s="11" t="s">
-        <v>914</v>
-      </c>
       <c r="D14" s="11" t="s">
-        <v>990</v>
+        <v>987</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="11" t="s">
-        <v>915</v>
+        <v>912</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>916</v>
+        <v>913</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>917</v>
+        <v>914</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>989</v>
+        <v>986</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
@@ -15798,10 +15802,10 @@
         <v>128</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>918</v>
+        <v>915</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>919</v>
+        <v>916</v>
       </c>
       <c r="D16" s="11" t="s">
         <v>874</v>
@@ -15809,13 +15813,13 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="11" t="s">
-        <v>920</v>
+        <v>917</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>921</v>
+        <v>918</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>922</v>
+        <v>919</v>
       </c>
       <c r="D17" s="11" t="s">
         <v>874</v>
@@ -15823,13 +15827,13 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" s="11" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>887</v>
+        <v>1162</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>888</v>
+        <v>1163</v>
       </c>
       <c r="D18" s="11" t="s">
         <v>874</v>
@@ -15837,13 +15841,13 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" s="11" t="s">
-        <v>923</v>
+        <v>920</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>924</v>
+        <v>921</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>925</v>
+        <v>922</v>
       </c>
       <c r="D19" s="11" t="s">
         <v>874</v>
@@ -15851,13 +15855,13 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" s="11" t="s">
-        <v>926</v>
+        <v>923</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>927</v>
+        <v>924</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>928</v>
+        <v>925</v>
       </c>
       <c r="D20" s="11" t="s">
         <v>874</v>
@@ -15865,13 +15869,13 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" s="11" t="s">
-        <v>929</v>
+        <v>926</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>930</v>
+        <v>927</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>931</v>
+        <v>928</v>
       </c>
       <c r="D21" s="11" t="s">
         <v>874</v>
@@ -15879,10 +15883,10 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" s="11" t="s">
-        <v>1024</v>
+        <v>1021</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>1025</v>
+        <v>1022</v>
       </c>
       <c r="C22" s="38" t="s">
         <v>463</v>
@@ -15893,13 +15897,13 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" s="11" t="s">
-        <v>932</v>
+        <v>929</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>933</v>
+        <v>930</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>934</v>
+        <v>931</v>
       </c>
       <c r="D23" s="11" t="s">
         <v>874</v>
@@ -15910,10 +15914,10 @@
         <v>351</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>935</v>
+        <v>932</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>936</v>
+        <v>933</v>
       </c>
       <c r="D24" s="11" t="s">
         <v>874</v>
@@ -15921,13 +15925,13 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" s="11" t="s">
-        <v>937</v>
+        <v>934</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>938</v>
+        <v>935</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>939</v>
+        <v>936</v>
       </c>
       <c r="D25" s="11" t="s">
         <v>874</v>
@@ -15935,13 +15939,13 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" s="11" t="s">
-        <v>943</v>
+        <v>940</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>944</v>
+        <v>941</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>945</v>
+        <v>942</v>
       </c>
       <c r="D26" s="11" t="s">
         <v>874</v>
@@ -15949,13 +15953,13 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" s="11" t="s">
-        <v>946</v>
+        <v>943</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>947</v>
+        <v>944</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>948</v>
+        <v>945</v>
       </c>
       <c r="D27" s="11" t="s">
         <v>874</v>
@@ -15974,7 +15978,7 @@
         <v>807</v>
       </c>
       <c r="D33" s="11" t="s">
-        <v>992</v>
+        <v>989</v>
       </c>
       <c r="E33" s="11" t="s">
         <v>875</v>
@@ -15988,7 +15992,7 @@
         <v>879</v>
       </c>
       <c r="D34" s="11" t="s">
-        <v>992</v>
+        <v>989</v>
       </c>
       <c r="E34" s="11" t="s">
         <v>880</v>
@@ -15996,30 +16000,30 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" s="11" t="s">
-        <v>889</v>
+        <v>886</v>
       </c>
       <c r="B35" s="11" t="s">
-        <v>890</v>
+        <v>887</v>
       </c>
       <c r="D35" s="11" t="s">
-        <v>992</v>
+        <v>989</v>
       </c>
       <c r="E35" s="11" t="s">
-        <v>891</v>
+        <v>888</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" s="11" t="s">
-        <v>940</v>
+        <v>937</v>
       </c>
       <c r="B36" s="11" t="s">
-        <v>941</v>
+        <v>938</v>
       </c>
       <c r="D36" s="11" t="s">
-        <v>992</v>
+        <v>989</v>
       </c>
       <c r="E36" s="11" t="s">
-        <v>942</v>
+        <v>939</v>
       </c>
     </row>
   </sheetData>
@@ -16028,9 +16032,10 @@
   </sortState>
   <hyperlinks>
     <hyperlink ref="C22" r:id="rId1" xr:uid="{A0A69456-20B2-498F-A811-8F2078E3E3EB}"/>
+    <hyperlink ref="C2" r:id="rId2" xr:uid="{E7B626A9-297F-40F7-9BC7-B7567E4CA15C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -16055,7 +16060,7 @@
   <sheetData>
     <row r="1" spans="1:4" s="45" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="45" t="s">
-        <v>1053</v>
+        <v>1050</v>
       </c>
       <c r="B1" s="45" t="s">
         <v>622</v>
@@ -16072,18 +16077,18 @@
         <v>10</v>
       </c>
       <c r="D2" s="44" t="s">
-        <v>966</v>
+        <v>963</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="44" t="s">
-        <v>957</v>
+        <v>954</v>
       </c>
       <c r="B3" s="44" t="s">
-        <v>958</v>
+        <v>955</v>
       </c>
       <c r="C3" s="44" t="s">
-        <v>959</v>
+        <v>956</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -16091,21 +16096,21 @@
         <v>629</v>
       </c>
       <c r="B4" s="44" t="s">
-        <v>967</v>
+        <v>964</v>
       </c>
       <c r="C4" s="44" t="s">
-        <v>968</v>
+        <v>965</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="44" t="s">
-        <v>960</v>
+        <v>957</v>
       </c>
       <c r="B5" s="44" t="s">
         <v>638</v>
       </c>
       <c r="C5" s="44" t="s">
-        <v>961</v>
+        <v>958</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -16113,10 +16118,10 @@
         <v>878</v>
       </c>
       <c r="B6" s="44" t="s">
-        <v>951</v>
+        <v>948</v>
       </c>
       <c r="C6" s="44" t="s">
-        <v>952</v>
+        <v>949</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -16124,10 +16129,10 @@
         <v>813</v>
       </c>
       <c r="B7" s="44" t="s">
-        <v>949</v>
+        <v>946</v>
       </c>
       <c r="C7" s="44" t="s">
-        <v>950</v>
+        <v>947</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -16138,40 +16143,40 @@
         <v>129</v>
       </c>
       <c r="D8" s="44" t="s">
-        <v>956</v>
+        <v>953</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="44" t="s">
-        <v>953</v>
+        <v>950</v>
       </c>
       <c r="B9" s="44" t="s">
-        <v>954</v>
+        <v>951</v>
       </c>
       <c r="C9" s="44" t="s">
-        <v>955</v>
+        <v>952</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="44" t="s">
-        <v>953</v>
+        <v>950</v>
       </c>
       <c r="B10" s="44" t="s">
-        <v>962</v>
+        <v>959</v>
       </c>
       <c r="C10" s="44" t="s">
-        <v>963</v>
+        <v>960</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="44" t="s">
-        <v>971</v>
+        <v>968</v>
       </c>
       <c r="B11" s="44" t="s">
-        <v>972</v>
+        <v>969</v>
       </c>
       <c r="C11" s="44" t="s">
-        <v>973</v>
+        <v>970</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -16179,15 +16184,15 @@
         <v>647</v>
       </c>
       <c r="B12" s="44" t="s">
-        <v>964</v>
+        <v>961</v>
       </c>
       <c r="C12" s="44" t="s">
-        <v>965</v>
+        <v>962</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="44" t="s">
-        <v>1023</v>
+        <v>1020</v>
       </c>
       <c r="B13" s="44" t="s">
         <v>386</v>
@@ -16203,21 +16208,21 @@
         <v>637</v>
       </c>
       <c r="B20" s="44" t="s">
-        <v>969</v>
+        <v>966</v>
       </c>
       <c r="D20" s="44" t="s">
-        <v>970</v>
+        <v>967</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="44" t="s">
-        <v>971</v>
+        <v>968</v>
       </c>
       <c r="B21" s="44" t="s">
-        <v>972</v>
+        <v>969</v>
       </c>
       <c r="D21" s="44" t="s">
-        <v>973</v>
+        <v>970</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
@@ -16225,21 +16230,21 @@
         <v>755</v>
       </c>
       <c r="B22" s="44" t="s">
-        <v>974</v>
+        <v>971</v>
       </c>
       <c r="D22" s="44" t="s">
-        <v>975</v>
+        <v>972</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="44" t="s">
-        <v>976</v>
+        <v>973</v>
       </c>
       <c r="B23" s="44" t="s">
-        <v>977</v>
+        <v>974</v>
       </c>
       <c r="D23" s="44" t="s">
-        <v>978</v>
+        <v>975</v>
       </c>
     </row>
   </sheetData>
@@ -16273,7 +16278,7 @@
   <sheetData>
     <row r="1" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="13" t="s">
-        <v>1053</v>
+        <v>1050</v>
       </c>
       <c r="B1" s="13" t="s">
         <v>1</v>
@@ -16282,10 +16287,10 @@
         <v>5</v>
       </c>
       <c r="D1" s="13" t="s">
-        <v>999</v>
+        <v>996</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>1000</v>
+        <v>997</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
@@ -16293,7 +16298,7 @@
         <v>30</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>1060</v>
+        <v>1057</v>
       </c>
       <c r="F2" s="11" t="s">
         <v>34</v>
@@ -16301,16 +16306,16 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="11" t="s">
-        <v>1066</v>
+        <v>1063</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>1067</v>
+        <v>1064</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>1072</v>
+        <v>1069</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>1044</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
@@ -16318,27 +16323,27 @@
         <v>9</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>1062</v>
+        <v>1059</v>
       </c>
       <c r="C4" s="38" t="s">
-        <v>1084</v>
+        <v>1081</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>1064</v>
+        <v>1061</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>1068</v>
+        <v>1065</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="11" t="s">
-        <v>1063</v>
+        <v>1060</v>
       </c>
       <c r="B5" s="11" t="s">
         <v>658</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>1065</v>
+        <v>1062</v>
       </c>
       <c r="D5" s="11" t="s">
         <v>161</v>
@@ -16349,13 +16354,13 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="11" t="s">
-        <v>1069</v>
+        <v>1066</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>1070</v>
+        <v>1067</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>1071</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
update Julia Morgan Building centenary agenda and resident directory
</commit_message>
<xml_diff>
--- a/3-1-heritage/0-heritage-happenings/2025/04-april-hh/resident-directory/2025-04-heritage-resident-directory.xlsx
+++ b/3-1-heritage/0-heritage-happenings/2025/04-april-hh/resident-directory/2025-04-heritage-resident-directory.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4348e1419f457eb2/Documents/GitHub/theo-armour-agenda/3-1-heritage/0-heritage-happenings/2025/04-april-hh/resident-directory/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="977" documentId="8_{47523533-A004-48EF-BEEC-0FA3DE3C4717}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1D5E067C-32C3-4A3F-B833-6A27FE94C34B}"/>
+  <xr:revisionPtr revIDLastSave="989" documentId="8_{47523533-A004-48EF-BEEC-0FA3DE3C4717}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F8422920-9A95-47B9-8B3E-0BAF306021ED}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="754" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1830" uniqueCount="1164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1838" uniqueCount="1172">
   <si>
     <t>First Name</t>
   </si>
@@ -3562,6 +3562,30 @@
   </si>
   <si>
     <t>&lt;rlochan@heritagesf.org&gt;</t>
+  </si>
+  <si>
+    <t>frank@rockwoodpacific.com</t>
+  </si>
+  <si>
+    <t>Frank</t>
+  </si>
+  <si>
+    <t>Rockwood</t>
+  </si>
+  <si>
+    <t>Carolyn</t>
+  </si>
+  <si>
+    <t>Kiernat</t>
+  </si>
+  <si>
+    <t>Kerri Young</t>
+  </si>
+  <si>
+    <t>kiernat@page-turnbull.com</t>
+  </si>
+  <si>
+    <t>kyoung@sfheritage.org</t>
   </si>
 </sst>
 </file>
@@ -4424,7 +4448,7 @@
   <dimension ref="A1:I1005"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A66" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F2" sqref="F2:F74"/>
     </sheetView>
   </sheetViews>
@@ -13225,11 +13249,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6F0A003-FE4F-475F-8A7A-E8033874D553}">
-  <dimension ref="A1:E100"/>
+  <dimension ref="A1:F100"/>
   <sheetViews>
     <sheetView showWhiteSpace="0" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2:C62"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23046875" defaultRowHeight="17.5" x14ac:dyDescent="0.35"/>
@@ -13242,7 +13266,7 @@
     <col min="6" max="16384" width="9.23046875" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="27" t="s">
         <v>1050</v>
       </c>
@@ -13259,7 +13283,7 @@
         <v>997</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="11" t="s">
         <v>625</v>
       </c>
@@ -13276,7 +13300,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="11" t="s">
         <v>748</v>
       </c>
@@ -13293,7 +13317,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="11" t="s">
         <v>634</v>
       </c>
@@ -13310,7 +13334,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="11" t="s">
         <v>637</v>
       </c>
@@ -13327,7 +13351,7 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="11" t="s">
         <v>187</v>
       </c>
@@ -13344,7 +13368,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="11" t="s">
         <v>641</v>
       </c>
@@ -13361,7 +13385,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="11" t="s">
         <v>643</v>
       </c>
@@ -13378,7 +13402,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="11" t="s">
         <v>645</v>
       </c>
@@ -13395,7 +13419,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="11" t="s">
         <v>647</v>
       </c>
@@ -13412,7 +13436,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="11" t="s">
         <v>649</v>
       </c>
@@ -13429,7 +13453,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="11" t="s">
         <v>651</v>
       </c>
@@ -13446,7 +13470,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="11" t="s">
         <v>723</v>
       </c>
@@ -13463,24 +13487,24 @@
         <v>166</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" s="11" t="s">
         <v>731</v>
       </c>
       <c r="B14" s="11" t="s">
         <v>732</v>
       </c>
-      <c r="C14" s="11" t="s">
-        <v>733</v>
-      </c>
       <c r="D14" s="8" t="s">
         <v>161</v>
       </c>
       <c r="E14" s="8" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F14" s="11" t="s">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="11" t="s">
         <v>726</v>
       </c>
@@ -13497,7 +13521,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" s="11" t="s">
         <v>175</v>
       </c>
@@ -14485,7 +14509,7 @@
   <dimension ref="A1:B37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
@@ -14802,8 +14826,8 @@
   <dimension ref="A1:C75"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C13" sqref="A13:C13"/>
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C3" sqref="C3:C75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23046875" defaultRowHeight="17.5" x14ac:dyDescent="0.35"/>
@@ -15571,11 +15595,11 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{125B352A-F0BB-4FBB-AB9A-46907AE2C1C2}">
-  <dimension ref="A1:E36"/>
+  <dimension ref="A1:E37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C27" sqref="C2:C27"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23046875" defaultRowHeight="17.5" x14ac:dyDescent="0.35"/>
@@ -15965,70 +15989,100 @@
         <v>874</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A32" s="13" t="s">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A29" s="11" t="s">
+        <v>1165</v>
+      </c>
+      <c r="B29" s="11" t="s">
+        <v>1166</v>
+      </c>
+      <c r="C29" s="11" t="s">
+        <v>1164</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A30" s="11" t="s">
+        <v>1167</v>
+      </c>
+      <c r="B30" s="11" t="s">
+        <v>1168</v>
+      </c>
+      <c r="C30" s="11" t="s">
+        <v>1170</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A31" s="11" t="s">
+        <v>1169</v>
+      </c>
+      <c r="C31" s="11" t="s">
+        <v>1171</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A33" s="13" t="s">
         <v>870</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A33" s="11" t="s">
-        <v>651</v>
-      </c>
-      <c r="B33" s="11" t="s">
-        <v>807</v>
-      </c>
-      <c r="D33" s="11" t="s">
-        <v>989</v>
-      </c>
-      <c r="E33" s="11" t="s">
-        <v>875</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" s="11" t="s">
-        <v>878</v>
+        <v>651</v>
       </c>
       <c r="B34" s="11" t="s">
-        <v>879</v>
+        <v>807</v>
       </c>
       <c r="D34" s="11" t="s">
         <v>989</v>
       </c>
       <c r="E34" s="11" t="s">
-        <v>880</v>
+        <v>875</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" s="11" t="s">
-        <v>886</v>
+        <v>878</v>
       </c>
       <c r="B35" s="11" t="s">
-        <v>887</v>
+        <v>879</v>
       </c>
       <c r="D35" s="11" t="s">
         <v>989</v>
       </c>
       <c r="E35" s="11" t="s">
-        <v>888</v>
+        <v>880</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" s="11" t="s">
-        <v>937</v>
+        <v>886</v>
       </c>
       <c r="B36" s="11" t="s">
-        <v>938</v>
+        <v>887</v>
       </c>
       <c r="D36" s="11" t="s">
         <v>989</v>
       </c>
       <c r="E36" s="11" t="s">
+        <v>888</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A37" s="11" t="s">
+        <v>937</v>
+      </c>
+      <c r="B37" s="11" t="s">
+        <v>938</v>
+      </c>
+      <c r="D37" s="11" t="s">
+        <v>989</v>
+      </c>
+      <c r="E37" s="11" t="s">
         <v>939</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E29">
-    <sortCondition ref="B2:B29"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E30">
+    <sortCondition ref="B2:B30"/>
   </sortState>
   <hyperlinks>
     <hyperlink ref="C22" r:id="rId1" xr:uid="{A0A69456-20B2-498F-A811-8F2078E3E3EB}"/>

</xml_diff>

<commit_message>
Add April 2025 resident directory and related documents
</commit_message>
<xml_diff>
--- a/3-1-heritage/0-heritage-happenings/2025/04-april-hh/resident-directory/2025-04-heritage-resident-directory.xlsx
+++ b/3-1-heritage/0-heritage-happenings/2025/04-april-hh/resident-directory/2025-04-heritage-resident-directory.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4348e1419f457eb2/Documents/GitHub/theo-armour-agenda/3-1-heritage/0-heritage-happenings/2025/04-april-hh/resident-directory/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="989" documentId="8_{47523533-A004-48EF-BEEC-0FA3DE3C4717}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F8422920-9A95-47B9-8B3E-0BAF306021ED}"/>
+  <xr:revisionPtr revIDLastSave="1006" documentId="8_{47523533-A004-48EF-BEEC-0FA3DE3C4717}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0E68DA9C-868D-48C7-8A07-0C40DF866C05}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="754" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="754" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Residents" sheetId="1" r:id="rId1"/>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1838" uniqueCount="1172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1844" uniqueCount="1177">
   <si>
     <t>First Name</t>
   </si>
@@ -3586,6 +3586,21 @@
   </si>
   <si>
     <t>kyoung@sfheritage.org</t>
+  </si>
+  <si>
+    <t>09/11</t>
+  </si>
+  <si>
+    <t>Carl Washington</t>
+  </si>
+  <si>
+    <t>415 792-6469</t>
+  </si>
+  <si>
+    <t>cwashington@allcovered.com</t>
+  </si>
+  <si>
+    <t>tessgoldman@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -4448,8 +4463,8 @@
   <dimension ref="A1:I1005"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F2" sqref="F2:F74"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.15234375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -4594,7 +4609,9 @@
       </c>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
-      <c r="I5" s="4"/>
+      <c r="I5" s="4" t="s">
+        <v>1172</v>
+      </c>
     </row>
     <row r="6" spans="1:9" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A6" s="17" t="s">
@@ -9138,6 +9155,9 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="86" fitToHeight="0" orientation="landscape" r:id="rId9"/>
+  <ignoredErrors>
+    <ignoredError sqref="I15" twoDigitTextYear="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
 
@@ -10078,8 +10098,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26C4F1CA-A107-47E1-B61D-684F7BB5060E}">
   <dimension ref="A1:Z173"/>
   <sheetViews>
-    <sheetView showGridLines="0" showZeros="0" showRuler="0" view="pageLayout" topLeftCell="A67" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A74" sqref="A2:A74"/>
+    <sheetView showGridLines="0" showZeros="0" tabSelected="1" showRuler="0" view="pageLayout" topLeftCell="A117" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D80" sqref="D80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.765625" defaultRowHeight="17.5" x14ac:dyDescent="0.35"/>
@@ -10166,20 +10186,20 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" s="11" t="str">
+      <c r="A5" s="43" t="str">
         <v>Jennifer Arthur</v>
       </c>
-      <c r="B5" s="11" t="str">
+      <c r="B5" s="43" t="str">
         <v>1530 Francisco</v>
       </c>
-      <c r="C5" s="11" t="str">
+      <c r="C5" s="43" t="str">
         <v>415-564-6616</v>
       </c>
-      <c r="D5" s="11" t="str">
+      <c r="D5" s="43" t="str">
         <v>jennifer@arthurassociates.net</v>
       </c>
-      <c r="E5" s="11">
-        <v>0</v>
+      <c r="E5" s="43" t="str">
+        <v>09/11</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
@@ -10577,7 +10597,7 @@
       <c r="A29" s="11" t="str">
         <v>Michele Jackson</v>
       </c>
-      <c r="B29" s="43" t="str">
+      <c r="B29" s="19" t="str">
         <v>1538 Francisco</v>
       </c>
       <c r="C29" s="11" t="str">
@@ -10798,7 +10818,7 @@
       <c r="A42" s="19" t="str">
         <v>Katie Loo</v>
       </c>
-      <c r="B42" s="43" t="str">
+      <c r="B42" s="19" t="str">
         <v>248 M</v>
       </c>
       <c r="C42" s="19" t="str">
@@ -10934,7 +10954,7 @@
       <c r="A50" s="11" t="str">
         <v>Anne Morris</v>
       </c>
-      <c r="B50" s="43" t="str">
+      <c r="B50" s="19" t="str">
         <v>324 M</v>
       </c>
       <c r="C50" s="11" t="str">
@@ -11396,54 +11416,71 @@
       <c r="D77" s="52"/>
       <c r="E77" s="52"/>
     </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A78" s="11" t="s">
+        <v>993</v>
+      </c>
+    </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A79" s="11" t="s">
-        <v>993</v>
+      <c r="A79" s="25" t="s">
+        <v>392</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A80" s="25" t="s">
-        <v>392</v>
-      </c>
+      <c r="A80" s="24" t="s">
+        <v>393</v>
+      </c>
+      <c r="B80" s="24"/>
+      <c r="C80" s="24"/>
+      <c r="D80" s="24"/>
+      <c r="E80" s="24"/>
     </row>
     <row r="81" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="A81" s="24" t="s">
-        <v>393</v>
-      </c>
-      <c r="B81" s="24"/>
-      <c r="C81" s="24"/>
-      <c r="D81" s="24"/>
-      <c r="E81" s="24"/>
-    </row>
-    <row r="82" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="A82" s="52" t="s">
+      <c r="A81" s="52" t="s">
         <v>1058</v>
       </c>
-      <c r="B82" s="52"/>
-      <c r="C82" s="52"/>
-      <c r="D82" s="52"/>
-      <c r="E82" s="52"/>
+      <c r="B81" s="52"/>
+      <c r="C81" s="52"/>
+      <c r="D81" s="52"/>
+      <c r="E81" s="52"/>
+    </row>
+    <row r="83" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A83" s="13" t="s">
+        <v>394</v>
+      </c>
+      <c r="B83" s="13" t="s">
+        <v>395</v>
+      </c>
+      <c r="C83" s="13" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="84" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="A84" s="13" t="s">
-        <v>394</v>
-      </c>
-      <c r="B84" s="13" t="s">
-        <v>395</v>
-      </c>
-      <c r="C84" s="13" t="s">
-        <v>4</v>
+      <c r="A84" s="19" t="s">
+        <v>396</v>
+      </c>
+      <c r="B84" s="19" t="s">
+        <v>397</v>
+      </c>
+      <c r="C84" s="19" t="s">
+        <v>398</v>
+      </c>
+      <c r="D84" s="11" t="s">
+        <v>1176</v>
       </c>
     </row>
     <row r="85" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="A85" s="19" t="s">
-        <v>396</v>
-      </c>
-      <c r="B85" s="19" t="s">
+      <c r="A85" s="11" t="s">
+        <v>1173</v>
+      </c>
+      <c r="B85" s="11" t="s">
         <v>397</v>
       </c>
-      <c r="C85" s="19" t="s">
-        <v>398</v>
+      <c r="C85" s="11" t="s">
+        <v>1174</v>
+      </c>
+      <c r="D85" s="11" t="s">
+        <v>1175</v>
       </c>
     </row>
     <row r="86" spans="1:26" x14ac:dyDescent="0.35">
@@ -12636,7 +12673,7 @@
   <pageSetup fitToHeight="0" orientation="landscape" r:id="rId2"/>
   <headerFooter>
     <oddHeader>&amp;L&amp;"-,Bold"&amp;14&amp;KC00000Heritage on the Marina&amp;R&amp;"-,Bold Italic"&amp;14&amp;KC00000Heritage Happenings Resident Directory</oddHeader>
-    <oddFooter>&amp;L&amp;14&amp;KC00000March 2025&amp;R&amp;14&amp;KC00000&amp;P</oddFooter>
+    <oddFooter>&amp;L&amp;14&amp;KC00000April 2025&amp;R&amp;14&amp;KC00000&amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -15597,7 +15634,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{125B352A-F0BB-4FBB-AB9A-46907AE2C1C2}">
   <dimension ref="A1:E37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C31" sqref="C31"/>
     </sheetView>

</xml_diff>

<commit_message>
Fix formatting in May newsletter for consistency
</commit_message>
<xml_diff>
--- a/3-1-heritage/0-heritage-happenings/2025/04-april-hh/resident-directory/2025-04-heritage-resident-directory.xlsx
+++ b/3-1-heritage/0-heritage-happenings/2025/04-april-hh/resident-directory/2025-04-heritage-resident-directory.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4348e1419f457eb2/Documents/GitHub/theo-armour-agenda/3-1-heritage/0-heritage-happenings/2025/04-april-hh/resident-directory/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1006" documentId="8_{47523533-A004-48EF-BEEC-0FA3DE3C4717}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0E68DA9C-868D-48C7-8A07-0C40DF866C05}"/>
+  <xr:revisionPtr revIDLastSave="1025" documentId="8_{47523533-A004-48EF-BEEC-0FA3DE3C4717}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6AF987C4-4644-488F-A1F4-BE6D7FF035B9}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="754" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="754" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Residents" sheetId="1" r:id="rId1"/>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1844" uniqueCount="1177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1857" uniqueCount="1190">
   <si>
     <t>First Name</t>
   </si>
@@ -3132,9 +3132,6 @@
     <t>Ernie's friend</t>
   </si>
   <si>
-    <t xml:space="preserve">Shirley </t>
-  </si>
-  <si>
     <t>Mary</t>
   </si>
   <si>
@@ -3579,9 +3576,6 @@
     <t>Kiernat</t>
   </si>
   <si>
-    <t>Kerri Young</t>
-  </si>
-  <si>
     <t>kiernat@page-turnbull.com</t>
   </si>
   <si>
@@ -3601,6 +3595,51 @@
   </si>
   <si>
     <t>tessgoldman@gmail.com</t>
+  </si>
+  <si>
+    <t>Young</t>
+  </si>
+  <si>
+    <t>Kerri</t>
+  </si>
+  <si>
+    <t>LD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ray's </t>
+  </si>
+  <si>
+    <t>phyllis17@gmail.com</t>
+  </si>
+  <si>
+    <t>Adam</t>
+  </si>
+  <si>
+    <t>abshaw98@gmail.com</t>
+  </si>
+  <si>
+    <t>Shaw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Carl </t>
+  </si>
+  <si>
+    <t>Washington</t>
+  </si>
+  <si>
+    <t>Phyllis</t>
+  </si>
+  <si>
+    <t>Wedvick</t>
+  </si>
+  <si>
+    <t>quincyeochilds@gmail.com</t>
+  </si>
+  <si>
+    <t>Quincy</t>
+  </si>
+  <si>
+    <t>Childs</t>
   </si>
 </sst>
 </file>
@@ -4463,8 +4502,8 @@
   <dimension ref="A1:I1005"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I15" sqref="I15"/>
+      <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F2" sqref="F2:F74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.15234375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -4482,7 +4521,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="17" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
       <c r="B1" s="17" t="s">
         <v>1</v>
@@ -4595,22 +4634,22 @@
         <v>778</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1" t="s">
         <v>38</v>
       </c>
       <c r="E5" s="1" t="s">
+        <v>1158</v>
+      </c>
+      <c r="F5" s="40" t="s">
         <v>1159</v>
-      </c>
-      <c r="F5" s="40" t="s">
-        <v>1160</v>
       </c>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
       <c r="I5" s="4" t="s">
-        <v>1172</v>
+        <v>1170</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="13.5" x14ac:dyDescent="0.3">
@@ -5232,7 +5271,7 @@
         <v>19</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>163</v>
@@ -5552,7 +5591,7 @@
         <v>19</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
       <c r="E43" s="1" t="s">
         <v>231</v>
@@ -5569,7 +5608,7 @@
     </row>
     <row r="44" spans="1:9" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A44" s="17" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="B44" s="17" t="s">
         <v>233</v>
@@ -5783,22 +5822,22 @@
     </row>
     <row r="53" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="17" t="s">
+        <v>1070</v>
+      </c>
+      <c r="B53" s="17" t="s">
         <v>1071</v>
       </c>
-      <c r="B53" s="17" t="s">
+      <c r="D53" s="1" t="s">
         <v>1072</v>
       </c>
-      <c r="D53" s="1" t="s">
+      <c r="E53" s="1" t="s">
         <v>1073</v>
       </c>
-      <c r="E53" s="1" t="s">
+      <c r="F53" s="39" t="s">
         <v>1074</v>
       </c>
-      <c r="F53" s="39" t="s">
+      <c r="I53" s="53" t="s">
         <v>1075</v>
-      </c>
-      <c r="I53" s="53" t="s">
-        <v>1076</v>
       </c>
     </row>
     <row r="54" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -5806,19 +5845,19 @@
         <v>843</v>
       </c>
       <c r="B54" s="17" t="s">
+        <v>1071</v>
+      </c>
+      <c r="D54" s="1" t="s">
         <v>1072</v>
       </c>
-      <c r="D54" s="1" t="s">
-        <v>1073</v>
-      </c>
       <c r="E54" s="1" t="s">
+        <v>1076</v>
+      </c>
+      <c r="F54" s="40" t="s">
+        <v>1079</v>
+      </c>
+      <c r="I54" s="53" t="s">
         <v>1077</v>
-      </c>
-      <c r="F54" s="40" t="s">
-        <v>1080</v>
-      </c>
-      <c r="I54" s="53" t="s">
-        <v>1078</v>
       </c>
     </row>
     <row r="55" spans="1:9" ht="13.5" x14ac:dyDescent="0.3">
@@ -5867,7 +5906,7 @@
         <v>288</v>
       </c>
       <c r="F56" s="49" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="G56" s="1"/>
       <c r="H56" s="1"/>
@@ -9210,7 +9249,7 @@
     </row>
     <row r="3" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>17</v>
@@ -10098,7 +10137,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26C4F1CA-A107-47E1-B61D-684F7BB5060E}">
   <dimension ref="A1:Z173"/>
   <sheetViews>
-    <sheetView showGridLines="0" showZeros="0" tabSelected="1" showRuler="0" view="pageLayout" topLeftCell="A117" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" showZeros="0" showRuler="0" view="pageLayout" topLeftCell="A117" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D80" sqref="D80"/>
     </sheetView>
   </sheetViews>
@@ -11437,7 +11476,7 @@
     </row>
     <row r="81" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A81" s="52" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
       <c r="B81" s="52"/>
       <c r="C81" s="52"/>
@@ -11466,21 +11505,21 @@
         <v>398</v>
       </c>
       <c r="D84" s="11" t="s">
-        <v>1176</v>
+        <v>1174</v>
       </c>
     </row>
     <row r="85" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A85" s="11" t="s">
-        <v>1173</v>
+        <v>1171</v>
       </c>
       <c r="B85" s="11" t="s">
         <v>397</v>
       </c>
       <c r="C85" s="11" t="s">
-        <v>1174</v>
+        <v>1172</v>
       </c>
       <c r="D85" s="11" t="s">
-        <v>1175</v>
+        <v>1173</v>
       </c>
     </row>
     <row r="86" spans="1:26" x14ac:dyDescent="0.35">
@@ -12693,7 +12732,7 @@
   <sheetData>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
       <c r="B2" t="s">
         <v>174</v>
@@ -12701,7 +12740,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
       <c r="B3" t="s">
         <v>174</v>
@@ -12709,7 +12748,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="B4" t="s">
         <v>174</v>
@@ -12717,7 +12756,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
       <c r="B5" t="s">
         <v>174</v>
@@ -12725,7 +12764,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
       <c r="B6" t="s">
         <v>110</v>
@@ -12733,7 +12772,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
       <c r="B7" t="s">
         <v>160</v>
@@ -12741,7 +12780,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
       <c r="B8" t="s">
         <v>132</v>
@@ -12749,7 +12788,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="B9" t="s">
         <v>301</v>
@@ -12757,7 +12796,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
       <c r="B10" t="s">
         <v>222</v>
@@ -12765,7 +12804,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="B11" t="s">
         <v>222</v>
@@ -12773,7 +12812,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
       <c r="B12" t="s">
         <v>35</v>
@@ -12781,15 +12820,15 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
       <c r="B13" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="B14" t="s">
         <v>127</v>
@@ -12797,7 +12836,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="B15" t="s">
         <v>127</v>
@@ -12805,7 +12844,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
       <c r="B16" t="s">
         <v>342</v>
@@ -12813,7 +12852,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="B17" t="s">
         <v>342</v>
@@ -12821,7 +12860,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="B18" t="s">
         <v>228</v>
@@ -12829,7 +12868,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
       <c r="B19" t="s">
         <v>208</v>
@@ -12837,7 +12876,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
       <c r="B20" t="s">
         <v>116</v>
@@ -12845,15 +12884,15 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
       <c r="B21" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="B22" t="s">
         <v>295</v>
@@ -12861,7 +12900,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="B23" t="s">
         <v>94</v>
@@ -12869,7 +12908,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
       <c r="B24" t="s">
         <v>62</v>
@@ -12877,7 +12916,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
       <c r="B25" t="s">
         <v>312</v>
@@ -12885,7 +12924,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="B26" t="s">
         <v>355</v>
@@ -12893,7 +12932,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="B27" t="s">
         <v>317</v>
@@ -12901,7 +12940,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="B28" t="s">
         <v>327</v>
@@ -12909,7 +12948,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
       <c r="B29" t="s">
         <v>289</v>
@@ -12917,7 +12956,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
       <c r="B30" t="s">
         <v>170</v>
@@ -12925,7 +12964,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
       <c r="B31" t="s">
         <v>186</v>
@@ -12933,7 +12972,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="B32" t="s">
         <v>369</v>
@@ -12941,7 +12980,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
       <c r="B33" t="s">
         <v>180</v>
@@ -12949,7 +12988,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
       <c r="B34" t="s">
         <v>84</v>
@@ -12957,7 +12996,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
       <c r="B35" t="s">
         <v>104</v>
@@ -12965,7 +13004,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="B36" t="s">
         <v>336</v>
@@ -12973,7 +13012,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
       <c r="B37" t="s">
         <v>135</v>
@@ -12981,7 +13020,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="B38" t="s">
         <v>147</v>
@@ -12989,7 +13028,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
       <c r="B39" t="s">
         <v>147</v>
@@ -12997,7 +13036,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
       <c r="B40" t="s">
         <v>381</v>
@@ -13005,7 +13044,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
       <c r="B41" t="s">
         <v>47</v>
@@ -13013,7 +13052,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
       <c r="B42" t="s">
         <v>268</v>
@@ -13021,7 +13060,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>1122</v>
+        <v>1121</v>
       </c>
       <c r="B43" t="s">
         <v>219</v>
@@ -13029,7 +13068,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
       <c r="B44" t="s">
         <v>213</v>
@@ -13037,7 +13076,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
       <c r="B45" t="s">
         <v>68</v>
@@ -13045,7 +13084,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="B46" t="s">
         <v>68</v>
@@ -13053,7 +13092,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="B47" t="s">
         <v>332</v>
@@ -13061,7 +13100,7 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
       <c r="B48" t="s">
         <v>252</v>
@@ -13069,7 +13108,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="B49" t="s">
         <v>16</v>
@@ -13077,7 +13116,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>1133</v>
+        <v>1132</v>
       </c>
       <c r="B50" t="s">
         <v>273</v>
@@ -13085,7 +13124,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
       <c r="B51" t="s">
         <v>79</v>
@@ -13093,7 +13132,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="B52" t="s">
         <v>29</v>
@@ -13101,7 +13140,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
       <c r="B53" t="s">
         <v>374</v>
@@ -13109,7 +13148,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
       <c r="B54" t="s">
         <v>192</v>
@@ -13117,7 +13156,7 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
       <c r="B55" t="s">
         <v>54</v>
@@ -13125,7 +13164,7 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
       <c r="B56" t="s">
         <v>54</v>
@@ -13133,7 +13172,7 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
       <c r="B57" t="s">
         <v>141</v>
@@ -13141,7 +13180,7 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="B58" t="s">
         <v>203</v>
@@ -13149,7 +13188,7 @@
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
       <c r="B59" t="s">
         <v>56</v>
@@ -13157,7 +13196,7 @@
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>1134</v>
+        <v>1133</v>
       </c>
       <c r="B60" t="s">
         <v>277</v>
@@ -13165,7 +13204,7 @@
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
       <c r="B61" t="s">
         <v>152</v>
@@ -13173,7 +13212,7 @@
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="B62" t="s">
         <v>154</v>
@@ -13181,7 +13220,7 @@
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
       <c r="B63" t="s">
         <v>122</v>
@@ -13189,7 +13228,7 @@
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
       <c r="B64" t="s">
         <v>41</v>
@@ -13197,7 +13236,7 @@
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
       <c r="B65" t="s">
         <v>385</v>
@@ -13205,7 +13244,7 @@
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
       <c r="B66" t="s">
         <v>306</v>
@@ -13213,7 +13252,7 @@
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>1130</v>
+        <v>1129</v>
       </c>
       <c r="B67" t="s">
         <v>257</v>
@@ -13221,7 +13260,7 @@
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="B68" t="s">
         <v>257</v>
@@ -13229,7 +13268,7 @@
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
       <c r="B69" t="s">
         <v>165</v>
@@ -13237,7 +13276,7 @@
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
       <c r="B70" t="s">
         <v>165</v>
@@ -13245,7 +13284,7 @@
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>1126</v>
+        <v>1125</v>
       </c>
       <c r="B71" t="s">
         <v>237</v>
@@ -13253,7 +13292,7 @@
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
       <c r="B72" t="s">
         <v>99</v>
@@ -13261,7 +13300,7 @@
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
       <c r="B73" t="s">
         <v>90</v>
@@ -13269,7 +13308,7 @@
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
       <c r="B74" t="s">
         <v>247</v>
@@ -13289,8 +13328,8 @@
   <dimension ref="A1:F100"/>
   <sheetViews>
     <sheetView showWhiteSpace="0" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F14" sqref="F14"/>
+      <pane ySplit="1" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="C2:C62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23046875" defaultRowHeight="17.5" x14ac:dyDescent="0.35"/>
@@ -13305,7 +13344,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="27" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
       <c r="B1" s="27" t="s">
         <v>995</v>
@@ -13342,13 +13381,13 @@
         <v>748</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
       <c r="E3" s="11" t="s">
         <v>25</v>
@@ -13713,13 +13752,13 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="38" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
       <c r="B25" s="38" t="s">
         <v>188</v>
       </c>
       <c r="C25" s="38" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="D25" s="19" t="s">
         <v>187</v>
@@ -13736,7 +13775,7 @@
         <v>188</v>
       </c>
       <c r="C26" s="38" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="D26" s="19" t="s">
         <v>187</v>
@@ -13832,16 +13871,16 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" s="11" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
       <c r="B32" s="11" t="s">
         <v>233</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
       <c r="D32" s="11" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="E32" s="11" t="s">
         <v>233</v>
@@ -13849,13 +13888,13 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" s="11" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="B33" s="11" t="s">
         <v>249</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="D33" s="11" t="s">
         <v>248</v>
@@ -13900,13 +13939,13 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" s="11" t="s">
+        <v>1033</v>
+      </c>
+      <c r="B36" s="11" t="s">
         <v>1034</v>
       </c>
-      <c r="B36" s="11" t="s">
+      <c r="C36" s="11" t="s">
         <v>1035</v>
-      </c>
-      <c r="C36" s="11" t="s">
-        <v>1036</v>
       </c>
       <c r="D36" s="11" t="s">
         <v>258</v>
@@ -14025,7 +14064,7 @@
         <v>1012</v>
       </c>
       <c r="C43" s="38" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="D43" s="11" t="s">
         <v>1003</v>
@@ -14144,7 +14183,7 @@
         <v>297</v>
       </c>
       <c r="C50" s="38" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
       <c r="D50" s="11" t="s">
         <v>296</v>
@@ -14746,7 +14785,7 @@
         <v>233</v>
       </c>
       <c r="B24" s="48" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
@@ -14860,11 +14899,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CAA4147-474C-47CD-A0DD-4C67000E8368}">
-  <dimension ref="A1:C75"/>
+  <dimension ref="A1:C83"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C3" sqref="C3:C75"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B83" sqref="B83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23046875" defaultRowHeight="17.5" x14ac:dyDescent="0.35"/>
@@ -14880,7 +14919,7 @@
   <sheetData>
     <row r="1" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="13" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
       <c r="B1" s="13" t="s">
         <v>622</v>
@@ -14946,7 +14985,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="8" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>31</v>
@@ -14979,7 +15018,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="11" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="B10" s="11" t="s">
         <v>743</v>
@@ -15554,7 +15593,7 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A70" s="11" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="B70" s="11" t="s">
         <v>741</v>
@@ -15565,57 +15604,122 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A71" s="11" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
       <c r="B71" s="11" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
       <c r="C71" s="11" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A72" s="11" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
       <c r="B72" s="11" t="s">
         <v>977</v>
       </c>
       <c r="C72" s="11" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A73" s="11" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="B73" s="11" t="s">
+        <v>1046</v>
+      </c>
+      <c r="C73" s="11" t="s">
         <v>1047</v>
-      </c>
-      <c r="C73" s="11" t="s">
-        <v>1048</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A74" s="11" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
       <c r="B74" s="11" t="s">
+        <v>1054</v>
+      </c>
+      <c r="C74" s="11" t="s">
         <v>1055</v>
-      </c>
-      <c r="C74" s="11" t="s">
-        <v>1056</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A75" s="11" t="s">
+        <v>1081</v>
+      </c>
+      <c r="B75" s="11" t="s">
         <v>1082</v>
       </c>
-      <c r="B75" s="11" t="s">
+      <c r="C75" s="11" t="s">
         <v>1083</v>
       </c>
-      <c r="C75" s="11" t="s">
-        <v>1084</v>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A76" s="11" t="s">
+        <v>1176</v>
+      </c>
+      <c r="B76" s="11" t="s">
+        <v>1175</v>
+      </c>
+      <c r="C76" s="11" t="s">
+        <v>1169</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A78" s="11" t="s">
+        <v>1177</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A79" s="11" t="s">
+        <v>1178</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A80" s="11" t="s">
+        <v>1185</v>
+      </c>
+      <c r="B80" s="11" t="s">
+        <v>1186</v>
+      </c>
+      <c r="C80" s="11" t="s">
+        <v>1179</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A81" s="11" t="s">
+        <v>1183</v>
+      </c>
+      <c r="B81" s="11" t="s">
+        <v>1184</v>
+      </c>
+      <c r="C81" s="11" t="s">
+        <v>1173</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A82" s="11" t="s">
+        <v>1180</v>
+      </c>
+      <c r="B82" s="11" t="s">
+        <v>1182</v>
+      </c>
+      <c r="C82" s="11" t="s">
+        <v>1181</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A83" s="11" t="s">
+        <v>1188</v>
+      </c>
+      <c r="B83" s="11" t="s">
+        <v>1189</v>
+      </c>
+      <c r="C83" s="11" t="s">
+        <v>1187</v>
       </c>
     </row>
   </sheetData>
@@ -15635,8 +15739,8 @@
   <dimension ref="A1:E37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C31" sqref="C31"/>
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="C2:C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23046875" defaultRowHeight="17.5" x14ac:dyDescent="0.35"/>
@@ -15650,7 +15754,7 @@
   <sheetData>
     <row r="1" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="13" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
       <c r="B1" s="13" t="s">
         <v>622</v>
@@ -15670,7 +15774,7 @@
         <v>882</v>
       </c>
       <c r="C2" s="38" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
       <c r="D2" s="11" t="s">
         <v>874</v>
@@ -15891,10 +15995,10 @@
         <v>885</v>
       </c>
       <c r="B18" s="11" t="s">
+        <v>1161</v>
+      </c>
+      <c r="C18" s="11" t="s">
         <v>1162</v>
-      </c>
-      <c r="C18" s="11" t="s">
-        <v>1163</v>
       </c>
       <c r="D18" s="11" t="s">
         <v>874</v>
@@ -15944,10 +16048,10 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" s="11" t="s">
+        <v>1020</v>
+      </c>
+      <c r="B22" s="11" t="s">
         <v>1021</v>
-      </c>
-      <c r="B22" s="11" t="s">
-        <v>1022</v>
       </c>
       <c r="C22" s="38" t="s">
         <v>463</v>
@@ -16028,32 +16132,24 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" s="11" t="s">
+        <v>1164</v>
+      </c>
+      <c r="B29" s="11" t="s">
         <v>1165</v>
       </c>
-      <c r="B29" s="11" t="s">
-        <v>1166</v>
-      </c>
       <c r="C29" s="11" t="s">
-        <v>1164</v>
+        <v>1163</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" s="11" t="s">
+        <v>1166</v>
+      </c>
+      <c r="B30" s="11" t="s">
         <v>1167</v>
       </c>
-      <c r="B30" s="11" t="s">
+      <c r="C30" s="11" t="s">
         <v>1168</v>
-      </c>
-      <c r="C30" s="11" t="s">
-        <v>1170</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A31" s="11" t="s">
-        <v>1169</v>
-      </c>
-      <c r="C31" s="11" t="s">
-        <v>1171</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
@@ -16151,7 +16247,7 @@
   <sheetData>
     <row r="1" spans="1:4" s="45" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="45" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
       <c r="B1" s="45" t="s">
         <v>622</v>
@@ -16279,14 +16375,6 @@
       </c>
       <c r="C12" s="44" t="s">
         <v>962</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="44" t="s">
-        <v>1020</v>
-      </c>
-      <c r="B13" s="44" t="s">
-        <v>386</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
@@ -16369,7 +16457,7 @@
   <sheetData>
     <row r="1" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="13" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
       <c r="B1" s="13" t="s">
         <v>1</v>
@@ -16389,7 +16477,7 @@
         <v>30</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
       <c r="F2" s="11" t="s">
         <v>34</v>
@@ -16397,16 +16485,16 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="11" t="s">
+        <v>1062</v>
+      </c>
+      <c r="B3" s="11" t="s">
         <v>1063</v>
       </c>
-      <c r="B3" s="11" t="s">
-        <v>1064</v>
-      </c>
       <c r="C3" s="11" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
@@ -16414,27 +16502,27 @@
         <v>9</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
       <c r="C4" s="38" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="11" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="B5" s="11" t="s">
         <v>658</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="D5" s="11" t="s">
         <v>161</v>
@@ -16445,13 +16533,13 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="11" t="s">
+        <v>1065</v>
+      </c>
+      <c r="B7" s="11" t="s">
         <v>1066</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="C7" s="11" t="s">
         <v>1067</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>1068</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Update personal agenda: remove outdated entries and add new items
</commit_message>
<xml_diff>
--- a/3-1-heritage/0-heritage-happenings/2025/04-april-hh/resident-directory/2025-04-heritage-resident-directory.xlsx
+++ b/3-1-heritage/0-heritage-happenings/2025/04-april-hh/resident-directory/2025-04-heritage-resident-directory.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4348e1419f457eb2/Documents/GitHub/theo-armour-agenda/3-1-heritage/0-heritage-happenings/2025/04-april-hh/resident-directory/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4348E1419F457EB2/Documents/GitHub/theo-armour-agenda/3-1-heritage/0-heritage-happenings/2025/04-april-hh/resident-directory/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1029" documentId="8_{47523533-A004-48EF-BEEC-0FA3DE3C4717}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0D2414A3-14C3-426F-A7C9-D70DDD6B0B09}"/>
+  <xr:revisionPtr revIDLastSave="1034" documentId="8_{47523533-A004-48EF-BEEC-0FA3DE3C4717}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A14B7B80-ABD6-4CEC-9F2E-A6E097A8AF1F}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="754" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1858" uniqueCount="1191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1858" uniqueCount="1190">
   <si>
     <t>First Name</t>
   </si>
@@ -2611,9 +2611,6 @@
   </si>
   <si>
     <t>Bennet</t>
-  </si>
-  <si>
-    <t>Englehardt</t>
   </si>
   <si>
     <t>&lt;bennet.engelhardt@gmail.com&gt;</t>
@@ -4524,7 +4521,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="17" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="B1" s="17" t="s">
         <v>1</v>
@@ -4637,22 +4634,22 @@
         <v>778</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1" t="s">
         <v>38</v>
       </c>
       <c r="E5" s="1" t="s">
+        <v>1157</v>
+      </c>
+      <c r="F5" s="40" t="s">
         <v>1158</v>
-      </c>
-      <c r="F5" s="40" t="s">
-        <v>1159</v>
       </c>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
       <c r="I5" s="4" t="s">
-        <v>1170</v>
+        <v>1169</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="13.5" x14ac:dyDescent="0.3">
@@ -5059,10 +5056,10 @@
     </row>
     <row r="22" spans="1:9" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A22" s="17" t="s">
+        <v>989</v>
+      </c>
+      <c r="B22" s="17" t="s">
         <v>990</v>
-      </c>
-      <c r="B22" s="17" t="s">
-        <v>991</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>19</v>
@@ -5071,10 +5068,10 @@
         <v>38</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="F22" s="40" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
@@ -5274,7 +5271,7 @@
         <v>19</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>163</v>
@@ -5594,7 +5591,7 @@
         <v>19</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
       <c r="E43" s="1" t="s">
         <v>231</v>
@@ -5611,7 +5608,7 @@
     </row>
     <row r="44" spans="1:9" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A44" s="17" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="B44" s="17" t="s">
         <v>233</v>
@@ -5825,22 +5822,22 @@
     </row>
     <row r="53" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="17" t="s">
+        <v>1069</v>
+      </c>
+      <c r="B53" s="17" t="s">
         <v>1070</v>
       </c>
-      <c r="B53" s="17" t="s">
+      <c r="D53" s="1" t="s">
         <v>1071</v>
       </c>
-      <c r="D53" s="1" t="s">
+      <c r="E53" s="1" t="s">
         <v>1072</v>
       </c>
-      <c r="E53" s="1" t="s">
+      <c r="F53" s="39" t="s">
         <v>1073</v>
       </c>
-      <c r="F53" s="39" t="s">
+      <c r="I53" s="53" t="s">
         <v>1074</v>
-      </c>
-      <c r="I53" s="53" t="s">
-        <v>1075</v>
       </c>
     </row>
     <row r="54" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -5848,19 +5845,19 @@
         <v>843</v>
       </c>
       <c r="B54" s="17" t="s">
+        <v>1070</v>
+      </c>
+      <c r="D54" s="1" t="s">
         <v>1071</v>
       </c>
-      <c r="D54" s="1" t="s">
-        <v>1072</v>
-      </c>
       <c r="E54" s="1" t="s">
+        <v>1075</v>
+      </c>
+      <c r="F54" s="40" t="s">
+        <v>1078</v>
+      </c>
+      <c r="I54" s="53" t="s">
         <v>1076</v>
-      </c>
-      <c r="F54" s="40" t="s">
-        <v>1079</v>
-      </c>
-      <c r="I54" s="53" t="s">
-        <v>1077</v>
       </c>
     </row>
     <row r="55" spans="1:9" ht="13.5" x14ac:dyDescent="0.3">
@@ -5909,7 +5906,7 @@
         <v>288</v>
       </c>
       <c r="F56" s="49" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
       <c r="G56" s="1"/>
       <c r="H56" s="1"/>
@@ -9252,7 +9249,7 @@
     </row>
     <row r="3" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>17</v>
@@ -11460,7 +11457,7 @@
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A78" s="11" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.35">
@@ -11479,7 +11476,7 @@
     </row>
     <row r="81" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A81" s="52" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
       <c r="B81" s="52"/>
       <c r="C81" s="52"/>
@@ -11508,21 +11505,21 @@
         <v>398</v>
       </c>
       <c r="D84" s="11" t="s">
-        <v>1174</v>
+        <v>1173</v>
       </c>
     </row>
     <row r="85" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A85" s="11" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
       <c r="B85" s="11" t="s">
         <v>397</v>
       </c>
       <c r="C85" s="11" t="s">
+        <v>1171</v>
+      </c>
+      <c r="D85" s="11" t="s">
         <v>1172</v>
-      </c>
-      <c r="D85" s="11" t="s">
-        <v>1173</v>
       </c>
     </row>
     <row r="86" spans="1:26" x14ac:dyDescent="0.35">
@@ -12735,7 +12732,7 @@
   <sheetData>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
       <c r="B2" t="s">
         <v>174</v>
@@ -12743,7 +12740,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
       <c r="B3" t="s">
         <v>174</v>
@@ -12751,7 +12748,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="B4" t="s">
         <v>174</v>
@@ -12759,7 +12756,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
       <c r="B5" t="s">
         <v>174</v>
@@ -12767,7 +12764,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
       <c r="B6" t="s">
         <v>110</v>
@@ -12775,7 +12772,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="B7" t="s">
         <v>160</v>
@@ -12783,7 +12780,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
       <c r="B8" t="s">
         <v>132</v>
@@ -12791,7 +12788,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="B9" t="s">
         <v>301</v>
@@ -12799,7 +12796,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>1122</v>
+        <v>1121</v>
       </c>
       <c r="B10" t="s">
         <v>222</v>
@@ -12807,7 +12804,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="B11" t="s">
         <v>222</v>
@@ -12815,7 +12812,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="B12" t="s">
         <v>35</v>
@@ -12823,15 +12820,15 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>1134</v>
+        <v>1133</v>
       </c>
       <c r="B13" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
       <c r="B14" t="s">
         <v>127</v>
@@ -12839,7 +12836,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="B15" t="s">
         <v>127</v>
@@ -12847,7 +12844,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="B16" t="s">
         <v>342</v>
@@ -12855,7 +12852,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="B17" t="s">
         <v>342</v>
@@ -12863,7 +12860,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
       <c r="B18" t="s">
         <v>228</v>
@@ -12871,7 +12868,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="B19" t="s">
         <v>208</v>
@@ -12879,7 +12876,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
       <c r="B20" t="s">
         <v>116</v>
@@ -12887,15 +12884,15 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
       <c r="B21" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
       <c r="B22" t="s">
         <v>295</v>
@@ -12903,7 +12900,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
       <c r="B23" t="s">
         <v>94</v>
@@ -12911,7 +12908,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
       <c r="B24" t="s">
         <v>62</v>
@@ -12919,7 +12916,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
       <c r="B25" t="s">
         <v>312</v>
@@ -12927,7 +12924,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="B26" t="s">
         <v>355</v>
@@ -12935,7 +12932,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
       <c r="B27" t="s">
         <v>317</v>
@@ -12943,7 +12940,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="B28" t="s">
         <v>327</v>
@@ -12951,7 +12948,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
       <c r="B29" t="s">
         <v>289</v>
@@ -12959,7 +12956,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
       <c r="B30" t="s">
         <v>170</v>
@@ -12967,7 +12964,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
       <c r="B31" t="s">
         <v>186</v>
@@ -12975,7 +12972,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="B32" t="s">
         <v>369</v>
@@ -12983,7 +12980,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
       <c r="B33" t="s">
         <v>180</v>
@@ -12991,7 +12988,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
       <c r="B34" t="s">
         <v>84</v>
@@ -12999,7 +12996,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
       <c r="B35" t="s">
         <v>104</v>
@@ -13007,7 +13004,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="B36" t="s">
         <v>336</v>
@@ -13015,7 +13012,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
       <c r="B37" t="s">
         <v>135</v>
@@ -13023,7 +13020,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
       <c r="B38" t="s">
         <v>147</v>
@@ -13031,7 +13028,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="B39" t="s">
         <v>147</v>
@@ -13039,7 +13036,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
       <c r="B40" t="s">
         <v>381</v>
@@ -13047,7 +13044,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
       <c r="B41" t="s">
         <v>47</v>
@@ -13055,7 +13052,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
       <c r="B42" t="s">
         <v>268</v>
@@ -13063,7 +13060,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
       <c r="B43" t="s">
         <v>219</v>
@@ -13071,7 +13068,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
       <c r="B44" t="s">
         <v>213</v>
@@ -13079,7 +13076,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
       <c r="B45" t="s">
         <v>68</v>
@@ -13087,7 +13084,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>1126</v>
+        <v>1125</v>
       </c>
       <c r="B46" t="s">
         <v>68</v>
@@ -13095,7 +13092,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="B47" t="s">
         <v>332</v>
@@ -13103,7 +13100,7 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
       <c r="B48" t="s">
         <v>252</v>
@@ -13111,7 +13108,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
       <c r="B49" t="s">
         <v>16</v>
@@ -13119,7 +13116,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
       <c r="B50" t="s">
         <v>273</v>
@@ -13127,7 +13124,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
       <c r="B51" t="s">
         <v>79</v>
@@ -13135,7 +13132,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="B52" t="s">
         <v>29</v>
@@ -13143,7 +13140,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="B53" t="s">
         <v>374</v>
@@ -13151,7 +13148,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
       <c r="B54" t="s">
         <v>192</v>
@@ -13159,7 +13156,7 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
       <c r="B55" t="s">
         <v>54</v>
@@ -13167,7 +13164,7 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
       <c r="B56" t="s">
         <v>54</v>
@@ -13175,7 +13172,7 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
       <c r="B57" t="s">
         <v>141</v>
@@ -13183,7 +13180,7 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
       <c r="B58" t="s">
         <v>203</v>
@@ -13191,7 +13188,7 @@
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
       <c r="B59" t="s">
         <v>56</v>
@@ -13199,7 +13196,7 @@
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>1133</v>
+        <v>1132</v>
       </c>
       <c r="B60" t="s">
         <v>277</v>
@@ -13207,7 +13204,7 @@
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="B61" t="s">
         <v>152</v>
@@ -13215,7 +13212,7 @@
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
       <c r="B62" t="s">
         <v>154</v>
@@ -13223,7 +13220,7 @@
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
       <c r="B63" t="s">
         <v>122</v>
@@ -13231,7 +13228,7 @@
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
       <c r="B64" t="s">
         <v>41</v>
@@ -13239,7 +13236,7 @@
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
       <c r="B65" t="s">
         <v>385</v>
@@ -13247,7 +13244,7 @@
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="B66" t="s">
         <v>306</v>
@@ -13255,7 +13252,7 @@
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
       <c r="B67" t="s">
         <v>257</v>
@@ -13263,7 +13260,7 @@
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="B68" t="s">
         <v>257</v>
@@ -13271,7 +13268,7 @@
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
       <c r="B69" t="s">
         <v>165</v>
@@ -13279,7 +13276,7 @@
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>1130</v>
+        <v>1129</v>
       </c>
       <c r="B70" t="s">
         <v>165</v>
@@ -13287,7 +13284,7 @@
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
       <c r="B71" t="s">
         <v>237</v>
@@ -13295,7 +13292,7 @@
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="B72" t="s">
         <v>99</v>
@@ -13303,7 +13300,7 @@
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
       <c r="B73" t="s">
         <v>90</v>
@@ -13311,7 +13308,7 @@
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="B74" t="s">
         <v>247</v>
@@ -13347,19 +13344,19 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="27" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="B1" s="27" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="C1" s="20" t="s">
         <v>5</v>
       </c>
       <c r="D1" s="27" t="s">
+        <v>995</v>
+      </c>
+      <c r="E1" s="27" t="s">
         <v>996</v>
-      </c>
-      <c r="E1" s="27" t="s">
-        <v>997</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
@@ -13384,13 +13381,13 @@
         <v>748</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="E3" s="11" t="s">
         <v>25</v>
@@ -13424,10 +13421,10 @@
         <v>639</v>
       </c>
       <c r="D5" s="11" t="s">
+        <v>1003</v>
+      </c>
+      <c r="E5" s="11" t="s">
         <v>1004</v>
-      </c>
-      <c r="E5" s="11" t="s">
-        <v>1005</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
@@ -13486,7 +13483,7 @@
         <v>645</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
       <c r="C9" s="19" t="s">
         <v>646</v>
@@ -13503,7 +13500,7 @@
         <v>647</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="C10" s="19" t="s">
         <v>648</v>
@@ -13543,7 +13540,7 @@
         <v>652</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="E12" s="11" t="s">
         <v>143</v>
@@ -13619,7 +13616,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="11" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="B17" s="11" t="s">
         <v>166</v>
@@ -13724,16 +13721,16 @@
         <v>661</v>
       </c>
       <c r="B23" s="11" t="s">
+        <v>998</v>
+      </c>
+      <c r="C23" s="19" t="s">
         <v>999</v>
-      </c>
-      <c r="C23" s="19" t="s">
-        <v>1000</v>
       </c>
       <c r="D23" s="11" t="s">
         <v>171</v>
       </c>
       <c r="E23" s="11" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
@@ -13741,7 +13738,7 @@
         <v>662</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="C24" s="19" t="s">
         <v>663</v>
@@ -13750,18 +13747,18 @@
         <v>171</v>
       </c>
       <c r="E24" s="11" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="38" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="B25" s="38" t="s">
         <v>188</v>
       </c>
       <c r="C25" s="38" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
       <c r="D25" s="19" t="s">
         <v>187</v>
@@ -13778,7 +13775,7 @@
         <v>188</v>
       </c>
       <c r="C26" s="38" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="D26" s="19" t="s">
         <v>187</v>
@@ -13792,7 +13789,7 @@
         <v>664</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="C27" s="19" t="s">
         <v>665</v>
@@ -13863,7 +13860,7 @@
         <v>230</v>
       </c>
       <c r="C31" s="19" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="D31" s="11" t="s">
         <v>229</v>
@@ -13874,16 +13871,16 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" s="11" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
       <c r="B32" s="11" t="s">
         <v>233</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
       <c r="D32" s="11" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="E32" s="11" t="s">
         <v>233</v>
@@ -13891,13 +13888,13 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" s="11" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="B33" s="11" t="s">
         <v>249</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="D33" s="11" t="s">
         <v>248</v>
@@ -13942,13 +13939,13 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" s="11" t="s">
+        <v>1032</v>
+      </c>
+      <c r="B36" s="11" t="s">
         <v>1033</v>
       </c>
-      <c r="B36" s="11" t="s">
+      <c r="C36" s="11" t="s">
         <v>1034</v>
-      </c>
-      <c r="C36" s="11" t="s">
-        <v>1035</v>
       </c>
       <c r="D36" s="11" t="s">
         <v>258</v>
@@ -14013,13 +14010,13 @@
         <v>684</v>
       </c>
       <c r="B40" s="11" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="C40" s="19" t="s">
         <v>685</v>
       </c>
       <c r="D40" s="11" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="E40" s="11" t="s">
         <v>270</v>
@@ -14036,7 +14033,7 @@
         <v>683</v>
       </c>
       <c r="D41" s="11" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="E41" s="11" t="s">
         <v>270</v>
@@ -14053,7 +14050,7 @@
         <v>682</v>
       </c>
       <c r="D42" s="11" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="E42" s="11" t="s">
         <v>270</v>
@@ -14064,13 +14061,13 @@
         <v>193</v>
       </c>
       <c r="B43" s="11" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="C43" s="38" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
       <c r="D43" s="11" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="E43" s="11" t="s">
         <v>270</v>
@@ -14121,7 +14118,7 @@
         <v>690</v>
       </c>
       <c r="D46" s="11" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="E46" s="11" t="s">
         <v>283</v>
@@ -14138,7 +14135,7 @@
         <v>692</v>
       </c>
       <c r="D47" s="11" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="E47" s="11" t="s">
         <v>283</v>
@@ -14149,13 +14146,13 @@
         <v>693</v>
       </c>
       <c r="B48" s="11" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="C48" s="19" t="s">
         <v>694</v>
       </c>
       <c r="D48" s="11" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="E48" s="11" t="s">
         <v>283</v>
@@ -14186,7 +14183,7 @@
         <v>297</v>
       </c>
       <c r="C50" s="38" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="D50" s="11" t="s">
         <v>296</v>
@@ -14217,7 +14214,7 @@
         <v>701</v>
       </c>
       <c r="B52" s="11" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
       <c r="C52" s="19" t="s">
         <v>702</v>
@@ -14231,7 +14228,7 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A53" s="11" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
       <c r="B53" s="11" t="s">
         <v>314</v>
@@ -14285,7 +14282,7 @@
         <v>706</v>
       </c>
       <c r="B56" s="11" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
       <c r="C56" s="19" t="s">
         <v>707</v>
@@ -14302,7 +14299,7 @@
         <v>804</v>
       </c>
       <c r="B57" s="11" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="C57" s="19" t="s">
         <v>705</v>
@@ -14356,10 +14353,10 @@
         <v>719</v>
       </c>
       <c r="C60" s="38" t="s">
+        <v>1005</v>
+      </c>
+      <c r="D60" s="11" t="s">
         <v>1006</v>
-      </c>
-      <c r="D60" s="11" t="s">
-        <v>1007</v>
       </c>
       <c r="E60" s="11" t="s">
         <v>376</v>
@@ -14376,7 +14373,7 @@
         <v>717</v>
       </c>
       <c r="D61" s="11" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
       <c r="E61" s="11" t="s">
         <v>376</v>
@@ -14393,7 +14390,7 @@
         <v>715</v>
       </c>
       <c r="D62" s="11" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
       <c r="E62" s="11" t="s">
         <v>376</v>
@@ -14788,7 +14785,7 @@
         <v>233</v>
       </c>
       <c r="B24" s="48" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
@@ -14905,8 +14902,8 @@
   <dimension ref="A1:E89"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D79" sqref="D79"/>
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C89" sqref="C89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23046875" defaultRowHeight="17.5" x14ac:dyDescent="0.35"/>
@@ -14922,7 +14919,7 @@
   <sheetData>
     <row r="1" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="13" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="B1" s="13" t="s">
         <v>622</v>
@@ -14933,24 +14930,24 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="11" t="s">
+        <v>851</v>
+      </c>
+      <c r="B2" s="11" t="s">
         <v>852</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="C2" s="11" t="s">
         <v>853</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>854</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="11" t="s">
+        <v>856</v>
+      </c>
+      <c r="B3" s="11" t="s">
         <v>857</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="C3" s="11" t="s">
         <v>858</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>859</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
@@ -14988,7 +14985,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="8" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>31</v>
@@ -15021,7 +15018,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="11" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="B10" s="11" t="s">
         <v>743</v>
@@ -15131,13 +15128,13 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="11" t="s">
+        <v>980</v>
+      </c>
+      <c r="B23" s="11" t="s">
         <v>981</v>
       </c>
-      <c r="B23" s="11" t="s">
+      <c r="C23" s="11" t="s">
         <v>982</v>
-      </c>
-      <c r="C23" s="11" t="s">
-        <v>983</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
@@ -15156,10 +15153,10 @@
         <v>815</v>
       </c>
       <c r="B25" s="11" t="s">
+        <v>854</v>
+      </c>
+      <c r="C25" s="11" t="s">
         <v>855</v>
-      </c>
-      <c r="C25" s="11" t="s">
-        <v>856</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
@@ -15200,10 +15197,10 @@
         <v>846</v>
       </c>
       <c r="B29" s="11" t="s">
+        <v>773</v>
+      </c>
+      <c r="C29" s="11" t="s">
         <v>847</v>
-      </c>
-      <c r="C29" s="11" t="s">
-        <v>848</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
@@ -15233,10 +15230,10 @@
         <v>793</v>
       </c>
       <c r="B32" s="11" t="s">
+        <v>859</v>
+      </c>
+      <c r="C32" s="11" t="s">
         <v>860</v>
-      </c>
-      <c r="C32" s="11" t="s">
-        <v>861</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
@@ -15318,13 +15315,13 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" s="11" t="s">
+        <v>866</v>
+      </c>
+      <c r="B41" s="11" t="s">
         <v>867</v>
       </c>
-      <c r="B41" s="11" t="s">
+      <c r="C41" s="11" t="s">
         <v>868</v>
-      </c>
-      <c r="C41" s="11" t="s">
-        <v>869</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.35">
@@ -15332,10 +15329,10 @@
         <v>672</v>
       </c>
       <c r="B42" s="11" t="s">
+        <v>983</v>
+      </c>
+      <c r="C42" s="11" t="s">
         <v>984</v>
-      </c>
-      <c r="C42" s="11" t="s">
-        <v>985</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.35">
@@ -15343,10 +15340,10 @@
         <v>651</v>
       </c>
       <c r="B43" s="11" t="s">
+        <v>862</v>
+      </c>
+      <c r="C43" s="11" t="s">
         <v>863</v>
-      </c>
-      <c r="C43" s="11" t="s">
-        <v>864</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.35">
@@ -15461,13 +15458,13 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A55" s="11" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="B55" s="11" t="s">
         <v>737</v>
       </c>
       <c r="C55" s="11" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.35">
@@ -15475,10 +15472,10 @@
         <v>755</v>
       </c>
       <c r="B56" s="11" t="s">
+        <v>978</v>
+      </c>
+      <c r="C56" s="8" t="s">
         <v>979</v>
-      </c>
-      <c r="C56" s="8" t="s">
-        <v>980</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.35">
@@ -15519,24 +15516,24 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A62" s="11" t="s">
+        <v>848</v>
+      </c>
+      <c r="B62" s="11" t="s">
         <v>849</v>
       </c>
-      <c r="B62" s="11" t="s">
+      <c r="C62" s="11" t="s">
         <v>850</v>
-      </c>
-      <c r="C62" s="11" t="s">
-        <v>851</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A63" s="11" t="s">
+        <v>975</v>
+      </c>
+      <c r="B63" s="11" t="s">
         <v>976</v>
       </c>
-      <c r="B63" s="11" t="s">
+      <c r="C63" s="19" t="s">
         <v>977</v>
-      </c>
-      <c r="C63" s="19" t="s">
-        <v>978</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.35">
@@ -15596,7 +15593,7 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A70" s="11" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
       <c r="B70" s="11" t="s">
         <v>741</v>
@@ -15607,137 +15604,137 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A71" s="11" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="B71" s="11" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
       <c r="C71" s="11" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A72" s="11" t="s">
+        <v>1043</v>
+      </c>
+      <c r="B72" s="11" t="s">
+        <v>976</v>
+      </c>
+      <c r="C72" s="11" t="s">
         <v>1044</v>
-      </c>
-      <c r="B72" s="11" t="s">
-        <v>977</v>
-      </c>
-      <c r="C72" s="11" t="s">
-        <v>1045</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A73" s="11" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
       <c r="B73" s="11" t="s">
+        <v>1045</v>
+      </c>
+      <c r="C73" s="11" t="s">
         <v>1046</v>
-      </c>
-      <c r="C73" s="11" t="s">
-        <v>1047</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A74" s="11" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
       <c r="B74" s="11" t="s">
+        <v>1053</v>
+      </c>
+      <c r="C74" s="11" t="s">
         <v>1054</v>
-      </c>
-      <c r="C74" s="11" t="s">
-        <v>1055</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A75" s="11" t="s">
+        <v>1080</v>
+      </c>
+      <c r="B75" s="11" t="s">
         <v>1081</v>
       </c>
-      <c r="B75" s="11" t="s">
+      <c r="C75" s="11" t="s">
         <v>1082</v>
-      </c>
-      <c r="C75" s="11" t="s">
-        <v>1083</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A76" s="11" t="s">
-        <v>1176</v>
+        <v>1175</v>
       </c>
       <c r="B76" s="11" t="s">
-        <v>1175</v>
+        <v>1174</v>
       </c>
       <c r="C76" s="11" t="s">
-        <v>1169</v>
+        <v>1168</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A78" s="11" t="s">
-        <v>1177</v>
+        <v>1176</v>
       </c>
       <c r="B78" s="11" t="s">
-        <v>1190</v>
+        <v>1189</v>
       </c>
       <c r="C78" s="11" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A80" s="11" t="s">
+        <v>1183</v>
+      </c>
+      <c r="B80" s="11" t="s">
         <v>1184</v>
       </c>
-      <c r="B80" s="11" t="s">
-        <v>1185</v>
-      </c>
       <c r="C80" s="11" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A81" s="11" t="s">
+        <v>1181</v>
+      </c>
+      <c r="B81" s="11" t="s">
         <v>1182</v>
       </c>
-      <c r="B81" s="11" t="s">
-        <v>1183</v>
-      </c>
       <c r="C81" s="11" t="s">
-        <v>1173</v>
+        <v>1172</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A82" s="11" t="s">
+        <v>1178</v>
+      </c>
+      <c r="B82" s="11" t="s">
+        <v>1180</v>
+      </c>
+      <c r="C82" s="11" t="s">
         <v>1179</v>
-      </c>
-      <c r="B82" s="11" t="s">
-        <v>1181</v>
-      </c>
-      <c r="C82" s="11" t="s">
-        <v>1180</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A83" s="11" t="s">
+        <v>1186</v>
+      </c>
+      <c r="B83" s="11" t="s">
         <v>1187</v>
       </c>
-      <c r="B83" s="11" t="s">
-        <v>1188</v>
-      </c>
       <c r="C83" s="11" t="s">
-        <v>1186</v>
+        <v>1185</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A85" s="11" t="s">
+        <v>1061</v>
+      </c>
+      <c r="B85" s="11" t="s">
         <v>1062</v>
       </c>
-      <c r="B85" s="11" t="s">
-        <v>1063</v>
-      </c>
       <c r="C85" s="11" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
       <c r="D85" s="11" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.35">
@@ -15745,27 +15742,27 @@
         <v>9</v>
       </c>
       <c r="B86" s="11" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
       <c r="C86" s="38" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
       <c r="D86" s="11" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="E86" s="11" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A87" s="11" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
       <c r="B87" s="11" t="s">
         <v>658</v>
       </c>
       <c r="C87" s="11" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
       <c r="D87" s="11" t="s">
         <v>161</v>
@@ -15776,13 +15773,13 @@
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A89" s="11" t="s">
+        <v>1064</v>
+      </c>
+      <c r="B89" s="11" t="s">
         <v>1065</v>
       </c>
-      <c r="B89" s="11" t="s">
+      <c r="C89" s="11" t="s">
         <v>1066</v>
-      </c>
-      <c r="C89" s="11" t="s">
-        <v>1067</v>
       </c>
     </row>
   </sheetData>
@@ -15818,7 +15815,7 @@
   <sheetData>
     <row r="1" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="13" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="B1" s="13" t="s">
         <v>622</v>
@@ -15832,30 +15829,30 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="11" t="s">
+        <v>880</v>
+      </c>
+      <c r="B2" s="11" t="s">
         <v>881</v>
       </c>
-      <c r="B2" s="11" t="s">
-        <v>882</v>
-      </c>
       <c r="C2" s="38" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="11" t="s">
+        <v>870</v>
+      </c>
+      <c r="B3" s="11" t="s">
         <v>871</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="C3" s="11" t="s">
         <v>872</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="D3" s="11" t="s">
         <v>873</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>874</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
@@ -15863,13 +15860,13 @@
         <v>748</v>
       </c>
       <c r="B4" s="11" t="s">
+        <v>875</v>
+      </c>
+      <c r="C4" s="11" t="s">
         <v>876</v>
       </c>
-      <c r="C4" s="11" t="s">
-        <v>877</v>
-      </c>
       <c r="D4" s="11" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
@@ -15877,55 +15874,55 @@
         <v>824</v>
       </c>
       <c r="B5" s="11" t="s">
+        <v>882</v>
+      </c>
+      <c r="C5" s="11" t="s">
         <v>883</v>
       </c>
-      <c r="C5" s="11" t="s">
-        <v>884</v>
-      </c>
       <c r="D5" s="11" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="11" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="B6" s="11" t="s">
+        <v>888</v>
+      </c>
+      <c r="C6" s="11" t="s">
         <v>889</v>
       </c>
-      <c r="C6" s="11" t="s">
-        <v>890</v>
-      </c>
       <c r="D6" s="11" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="11" t="s">
+        <v>890</v>
+      </c>
+      <c r="B7" s="11" t="s">
         <v>891</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="C7" s="11" t="s">
         <v>892</v>
       </c>
-      <c r="C7" s="11" t="s">
-        <v>893</v>
-      </c>
       <c r="D7" s="11" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="11" t="s">
+        <v>893</v>
+      </c>
+      <c r="B8" s="11" t="s">
         <v>894</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="C8" s="11" t="s">
         <v>895</v>
       </c>
-      <c r="C8" s="11" t="s">
-        <v>896</v>
-      </c>
       <c r="D8" s="11" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
@@ -15933,55 +15930,55 @@
         <v>48</v>
       </c>
       <c r="B9" s="11" t="s">
+        <v>896</v>
+      </c>
+      <c r="C9" s="11" t="s">
         <v>897</v>
       </c>
-      <c r="C9" s="11" t="s">
-        <v>898</v>
-      </c>
       <c r="D9" s="11" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="11" t="s">
+        <v>898</v>
+      </c>
+      <c r="B10" s="11" t="s">
         <v>899</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="C10" s="11" t="s">
         <v>900</v>
       </c>
-      <c r="C10" s="11" t="s">
-        <v>901</v>
-      </c>
       <c r="D10" s="11" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="11" t="s">
+        <v>901</v>
+      </c>
+      <c r="B11" s="11" t="s">
         <v>902</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="C11" s="11" t="s">
         <v>903</v>
       </c>
-      <c r="C11" s="11" t="s">
-        <v>904</v>
-      </c>
       <c r="D11" s="11" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="11" t="s">
+        <v>904</v>
+      </c>
+      <c r="B12" s="11" t="s">
         <v>905</v>
       </c>
-      <c r="B12" s="11" t="s">
+      <c r="C12" s="11" t="s">
         <v>906</v>
       </c>
-      <c r="C12" s="11" t="s">
-        <v>907</v>
-      </c>
       <c r="D12" s="11" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
@@ -15989,41 +15986,41 @@
         <v>755</v>
       </c>
       <c r="B13" s="11" t="s">
+        <v>907</v>
+      </c>
+      <c r="C13" s="11" t="s">
         <v>908</v>
       </c>
-      <c r="C13" s="11" t="s">
-        <v>909</v>
-      </c>
       <c r="D13" s="11" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="11" t="s">
+        <v>909</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>907</v>
+      </c>
+      <c r="C14" s="11" t="s">
         <v>910</v>
       </c>
-      <c r="B14" s="11" t="s">
-        <v>908</v>
-      </c>
-      <c r="C14" s="11" t="s">
-        <v>911</v>
-      </c>
       <c r="D14" s="11" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="11" t="s">
+        <v>911</v>
+      </c>
+      <c r="B15" s="11" t="s">
         <v>912</v>
       </c>
-      <c r="B15" s="11" t="s">
+      <c r="C15" s="11" t="s">
         <v>913</v>
       </c>
-      <c r="C15" s="11" t="s">
-        <v>914</v>
-      </c>
       <c r="D15" s="11" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
@@ -16031,111 +16028,111 @@
         <v>128</v>
       </c>
       <c r="B16" s="11" t="s">
+        <v>914</v>
+      </c>
+      <c r="C16" s="11" t="s">
         <v>915</v>
       </c>
-      <c r="C16" s="11" t="s">
-        <v>916</v>
-      </c>
       <c r="D16" s="11" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="11" t="s">
+        <v>916</v>
+      </c>
+      <c r="B17" s="11" t="s">
         <v>917</v>
       </c>
-      <c r="B17" s="11" t="s">
+      <c r="C17" s="11" t="s">
         <v>918</v>
       </c>
-      <c r="C17" s="11" t="s">
-        <v>919</v>
-      </c>
       <c r="D17" s="11" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" s="11" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="B18" s="11" t="s">
+        <v>1160</v>
+      </c>
+      <c r="C18" s="11" t="s">
         <v>1161</v>
       </c>
-      <c r="C18" s="11" t="s">
-        <v>1162</v>
-      </c>
       <c r="D18" s="11" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" s="11" t="s">
+        <v>919</v>
+      </c>
+      <c r="B19" s="11" t="s">
         <v>920</v>
       </c>
-      <c r="B19" s="11" t="s">
+      <c r="C19" s="11" t="s">
         <v>921</v>
       </c>
-      <c r="C19" s="11" t="s">
-        <v>922</v>
-      </c>
       <c r="D19" s="11" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" s="11" t="s">
+        <v>922</v>
+      </c>
+      <c r="B20" s="11" t="s">
         <v>923</v>
       </c>
-      <c r="B20" s="11" t="s">
+      <c r="C20" s="11" t="s">
         <v>924</v>
       </c>
-      <c r="C20" s="11" t="s">
-        <v>925</v>
-      </c>
       <c r="D20" s="11" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" s="11" t="s">
+        <v>925</v>
+      </c>
+      <c r="B21" s="11" t="s">
         <v>926</v>
       </c>
-      <c r="B21" s="11" t="s">
+      <c r="C21" s="11" t="s">
         <v>927</v>
       </c>
-      <c r="C21" s="11" t="s">
-        <v>928</v>
-      </c>
       <c r="D21" s="11" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" s="11" t="s">
+        <v>1019</v>
+      </c>
+      <c r="B22" s="11" t="s">
         <v>1020</v>
-      </c>
-      <c r="B22" s="11" t="s">
-        <v>1021</v>
       </c>
       <c r="C22" s="38" t="s">
         <v>463</v>
       </c>
       <c r="D22" s="11" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" s="11" t="s">
+        <v>928</v>
+      </c>
+      <c r="B23" s="11" t="s">
         <v>929</v>
       </c>
-      <c r="B23" s="11" t="s">
+      <c r="C23" s="11" t="s">
         <v>930</v>
       </c>
-      <c r="C23" s="11" t="s">
-        <v>931</v>
-      </c>
       <c r="D23" s="11" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
@@ -16143,82 +16140,82 @@
         <v>351</v>
       </c>
       <c r="B24" s="11" t="s">
+        <v>931</v>
+      </c>
+      <c r="C24" s="11" t="s">
         <v>932</v>
       </c>
-      <c r="C24" s="11" t="s">
-        <v>933</v>
-      </c>
       <c r="D24" s="11" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" s="11" t="s">
+        <v>933</v>
+      </c>
+      <c r="B25" s="11" t="s">
         <v>934</v>
       </c>
-      <c r="B25" s="11" t="s">
+      <c r="C25" s="11" t="s">
         <v>935</v>
       </c>
-      <c r="C25" s="11" t="s">
-        <v>936</v>
-      </c>
       <c r="D25" s="11" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" s="11" t="s">
+        <v>939</v>
+      </c>
+      <c r="B26" s="11" t="s">
         <v>940</v>
       </c>
-      <c r="B26" s="11" t="s">
+      <c r="C26" s="11" t="s">
         <v>941</v>
       </c>
-      <c r="C26" s="11" t="s">
-        <v>942</v>
-      </c>
       <c r="D26" s="11" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" s="11" t="s">
+        <v>942</v>
+      </c>
+      <c r="B27" s="11" t="s">
         <v>943</v>
       </c>
-      <c r="B27" s="11" t="s">
+      <c r="C27" s="11" t="s">
         <v>944</v>
       </c>
-      <c r="C27" s="11" t="s">
-        <v>945</v>
-      </c>
       <c r="D27" s="11" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" s="11" t="s">
+        <v>1163</v>
+      </c>
+      <c r="B29" s="11" t="s">
         <v>1164</v>
       </c>
-      <c r="B29" s="11" t="s">
-        <v>1165</v>
-      </c>
       <c r="C29" s="11" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" s="11" t="s">
+        <v>1165</v>
+      </c>
+      <c r="B30" s="11" t="s">
         <v>1166</v>
       </c>
-      <c r="B30" s="11" t="s">
+      <c r="C30" s="11" t="s">
         <v>1167</v>
-      </c>
-      <c r="C30" s="11" t="s">
-        <v>1168</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" s="13" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.35">
@@ -16229,52 +16226,52 @@
         <v>807</v>
       </c>
       <c r="D34" s="11" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
       <c r="E34" s="11" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" s="11" t="s">
+        <v>877</v>
+      </c>
+      <c r="B35" s="11" t="s">
         <v>878</v>
       </c>
-      <c r="B35" s="11" t="s">
+      <c r="D35" s="11" t="s">
+        <v>988</v>
+      </c>
+      <c r="E35" s="11" t="s">
         <v>879</v>
-      </c>
-      <c r="D35" s="11" t="s">
-        <v>989</v>
-      </c>
-      <c r="E35" s="11" t="s">
-        <v>880</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" s="11" t="s">
+        <v>885</v>
+      </c>
+      <c r="B36" s="11" t="s">
         <v>886</v>
       </c>
-      <c r="B36" s="11" t="s">
+      <c r="D36" s="11" t="s">
+        <v>988</v>
+      </c>
+      <c r="E36" s="11" t="s">
         <v>887</v>
-      </c>
-      <c r="D36" s="11" t="s">
-        <v>989</v>
-      </c>
-      <c r="E36" s="11" t="s">
-        <v>888</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" s="11" t="s">
+        <v>936</v>
+      </c>
+      <c r="B37" s="11" t="s">
         <v>937</v>
       </c>
-      <c r="B37" s="11" t="s">
+      <c r="D37" s="11" t="s">
+        <v>988</v>
+      </c>
+      <c r="E37" s="11" t="s">
         <v>938</v>
-      </c>
-      <c r="D37" s="11" t="s">
-        <v>989</v>
-      </c>
-      <c r="E37" s="11" t="s">
-        <v>939</v>
       </c>
     </row>
   </sheetData>
@@ -16311,7 +16308,7 @@
   <sheetData>
     <row r="1" spans="1:4" s="45" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="45" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="B1" s="45" t="s">
         <v>622</v>
@@ -16328,18 +16325,18 @@
         <v>10</v>
       </c>
       <c r="D2" s="44" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="44" t="s">
+        <v>953</v>
+      </c>
+      <c r="B3" s="44" t="s">
         <v>954</v>
       </c>
-      <c r="B3" s="44" t="s">
+      <c r="C3" s="44" t="s">
         <v>955</v>
-      </c>
-      <c r="C3" s="44" t="s">
-        <v>956</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -16347,32 +16344,32 @@
         <v>629</v>
       </c>
       <c r="B4" s="44" t="s">
+        <v>963</v>
+      </c>
+      <c r="C4" s="44" t="s">
         <v>964</v>
-      </c>
-      <c r="C4" s="44" t="s">
-        <v>965</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="44" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="B5" s="44" t="s">
         <v>638</v>
       </c>
       <c r="C5" s="44" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="44" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="B6" s="44" t="s">
+        <v>947</v>
+      </c>
+      <c r="C6" s="44" t="s">
         <v>948</v>
-      </c>
-      <c r="C6" s="44" t="s">
-        <v>949</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -16380,10 +16377,10 @@
         <v>813</v>
       </c>
       <c r="B7" s="44" t="s">
+        <v>945</v>
+      </c>
+      <c r="C7" s="44" t="s">
         <v>946</v>
-      </c>
-      <c r="C7" s="44" t="s">
-        <v>947</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -16394,40 +16391,40 @@
         <v>129</v>
       </c>
       <c r="D8" s="44" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="44" t="s">
+        <v>949</v>
+      </c>
+      <c r="B9" s="44" t="s">
         <v>950</v>
       </c>
-      <c r="B9" s="44" t="s">
+      <c r="C9" s="44" t="s">
         <v>951</v>
-      </c>
-      <c r="C9" s="44" t="s">
-        <v>952</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="44" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
       <c r="B10" s="44" t="s">
+        <v>958</v>
+      </c>
+      <c r="C10" s="44" t="s">
         <v>959</v>
-      </c>
-      <c r="C10" s="44" t="s">
-        <v>960</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="44" t="s">
+        <v>967</v>
+      </c>
+      <c r="B11" s="44" t="s">
         <v>968</v>
       </c>
-      <c r="B11" s="44" t="s">
+      <c r="C11" s="44" t="s">
         <v>969</v>
-      </c>
-      <c r="C11" s="44" t="s">
-        <v>970</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -16435,15 +16432,15 @@
         <v>647</v>
       </c>
       <c r="B12" s="44" t="s">
+        <v>960</v>
+      </c>
+      <c r="C12" s="44" t="s">
         <v>961</v>
-      </c>
-      <c r="C12" s="44" t="s">
-        <v>962</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="45" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
@@ -16451,21 +16448,21 @@
         <v>637</v>
       </c>
       <c r="B20" s="44" t="s">
+        <v>965</v>
+      </c>
+      <c r="D20" s="44" t="s">
         <v>966</v>
-      </c>
-      <c r="D20" s="44" t="s">
-        <v>967</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="44" t="s">
+        <v>967</v>
+      </c>
+      <c r="B21" s="44" t="s">
         <v>968</v>
       </c>
-      <c r="B21" s="44" t="s">
+      <c r="D21" s="44" t="s">
         <v>969</v>
-      </c>
-      <c r="D21" s="44" t="s">
-        <v>970</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
@@ -16473,21 +16470,21 @@
         <v>755</v>
       </c>
       <c r="B22" s="44" t="s">
+        <v>970</v>
+      </c>
+      <c r="D22" s="44" t="s">
         <v>971</v>
-      </c>
-      <c r="D22" s="44" t="s">
-        <v>972</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="44" t="s">
+        <v>972</v>
+      </c>
+      <c r="B23" s="44" t="s">
         <v>973</v>
       </c>
-      <c r="B23" s="44" t="s">
+      <c r="D23" s="44" t="s">
         <v>974</v>
-      </c>
-      <c r="D23" s="44" t="s">
-        <v>975</v>
       </c>
     </row>
   </sheetData>
@@ -16521,7 +16518,7 @@
   <sheetData>
     <row r="1" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="13" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="B1" s="13" t="s">
         <v>1</v>
@@ -16530,10 +16527,10 @@
         <v>5</v>
       </c>
       <c r="D1" s="13" t="s">
+        <v>995</v>
+      </c>
+      <c r="E1" s="13" t="s">
         <v>996</v>
-      </c>
-      <c r="E1" s="13" t="s">
-        <v>997</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
@@ -16541,7 +16538,7 @@
         <v>30</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="F2" s="11" t="s">
         <v>34</v>

</xml_diff>